<commit_message>
Age changed to timestamp - adjust feature selection
Feature selection will now only delete numerical features
</commit_message>
<xml_diff>
--- a/Data_summary.xlsx
+++ b/Data_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="68">
   <si>
     <t>subjectLabel</t>
   </si>
@@ -198,11 +198,35 @@
   <si>
     <t>Children_C37</t>
   </si>
+  <si>
+    <t>Adults_B1</t>
+  </si>
+  <si>
+    <t>Adults_G2</t>
+  </si>
+  <si>
+    <t>Adults_B2</t>
+  </si>
+  <si>
+    <t>Adults_G3</t>
+  </si>
+  <si>
+    <t>Adults_G4</t>
+  </si>
+  <si>
+    <t>Adults_B3</t>
+  </si>
+  <si>
+    <t>Adults_G6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -255,11 +279,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN288"/>
+  <dimension ref="A1:AN326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -35414,6 +35439,4642 @@
         <v>0</v>
       </c>
     </row>
+    <row r="289" spans="1:40">
+      <c r="A289" s="1">
+        <v>0</v>
+      </c>
+      <c r="B289" t="s">
+        <v>61</v>
+      </c>
+      <c r="C289">
+        <v>699</v>
+      </c>
+      <c r="D289">
+        <v>11</v>
+      </c>
+      <c r="E289">
+        <v>62.50943217710424</v>
+      </c>
+      <c r="F289">
+        <v>150.0358636476149</v>
+      </c>
+      <c r="G289">
+        <v>-7.700503917289078</v>
+      </c>
+      <c r="H289">
+        <v>68.48078481776818</v>
+      </c>
+      <c r="I289">
+        <v>4689.617889257469</v>
+      </c>
+      <c r="J289">
+        <v>24.48904267229756</v>
+      </c>
+      <c r="K289">
+        <v>59.67139684159727</v>
+      </c>
+      <c r="L289">
+        <v>0.4097187187054203</v>
+      </c>
+      <c r="M289">
+        <v>26.51083286537076</v>
+      </c>
+      <c r="N289">
+        <v>702.8242592156221</v>
+      </c>
+      <c r="O289">
+        <v>0.238701139104487</v>
+      </c>
+      <c r="P289">
+        <v>11.20286649197953</v>
+      </c>
+      <c r="Q289">
+        <v>-1.531326439728364</v>
+      </c>
+      <c r="R289">
+        <v>1.399206541166576</v>
+      </c>
+      <c r="S289">
+        <v>1.957778944843332</v>
+      </c>
+      <c r="T289">
+        <v>0.1159941200901191</v>
+      </c>
+      <c r="U289">
+        <v>2.623331004827961</v>
+      </c>
+      <c r="V289">
+        <v>-0.8276605610887984</v>
+      </c>
+      <c r="W289">
+        <v>0.4503335429616671</v>
+      </c>
+      <c r="X289">
+        <v>0.2028002999164077</v>
+      </c>
+      <c r="Y289">
+        <v>49.3199940679917</v>
+      </c>
+      <c r="Z289">
+        <v>10.10342263550179</v>
+      </c>
+      <c r="AA289">
+        <v>15.17951909646679</v>
+      </c>
+      <c r="AB289">
+        <v>0</v>
+      </c>
+      <c r="AC289">
+        <v>1.075018874061645</v>
+      </c>
+      <c r="AD289">
+        <v>-0.3663759238635719</v>
+      </c>
+      <c r="AE289">
+        <v>364.6300817711557</v>
+      </c>
+      <c r="AF289">
+        <v>-533.7512251793203</v>
+      </c>
+      <c r="AG289">
+        <v>63.95275219106426</v>
+      </c>
+      <c r="AH289">
+        <v>20.83119875911411</v>
+      </c>
+      <c r="AI289">
+        <v>-1.033751876865415</v>
+      </c>
+      <c r="AJ289">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK289">
+        <v>0.002</v>
+      </c>
+      <c r="AL289">
+        <v>0.002</v>
+      </c>
+      <c r="AM289" s="2">
+        <v>37527</v>
+      </c>
+      <c r="AN289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:40">
+      <c r="A290" s="1">
+        <v>0</v>
+      </c>
+      <c r="B290" t="s">
+        <v>61</v>
+      </c>
+      <c r="C290">
+        <v>699</v>
+      </c>
+      <c r="D290">
+        <v>11</v>
+      </c>
+      <c r="E290">
+        <v>119.5617186924291</v>
+      </c>
+      <c r="F290">
+        <v>128.6572975501379</v>
+      </c>
+      <c r="G290">
+        <v>106.5182493958348</v>
+      </c>
+      <c r="H290">
+        <v>4.706298193877228</v>
+      </c>
+      <c r="I290">
+        <v>22.14924268969206</v>
+      </c>
+      <c r="J290">
+        <v>57.84331426678359</v>
+      </c>
+      <c r="K290">
+        <v>63.22901671793025</v>
+      </c>
+      <c r="L290">
+        <v>52.0856854874479</v>
+      </c>
+      <c r="M290">
+        <v>1.460527801597048</v>
+      </c>
+      <c r="N290">
+        <v>2.133141459237906</v>
+      </c>
+      <c r="O290">
+        <v>0.009090112512271851</v>
+      </c>
+      <c r="P290">
+        <v>1.265016341016661</v>
+      </c>
+      <c r="Q290">
+        <v>-1.356854043963438</v>
+      </c>
+      <c r="R290">
+        <v>0.4357988916558875</v>
+      </c>
+      <c r="S290">
+        <v>0.1899206739685</v>
+      </c>
+      <c r="T290">
+        <v>-0.001738894967617173</v>
+      </c>
+      <c r="U290">
+        <v>1.562669589639832</v>
+      </c>
+      <c r="V290">
+        <v>-1.424074263249878</v>
+      </c>
+      <c r="W290">
+        <v>0.4198226952133804</v>
+      </c>
+      <c r="X290">
+        <v>0.1762510954162269</v>
+      </c>
+      <c r="Y290">
+        <v>58.2138967634892</v>
+      </c>
+      <c r="Z290">
+        <v>9.997122580799472</v>
+      </c>
+      <c r="AA290">
+        <v>13.77196064473029</v>
+      </c>
+      <c r="AB290">
+        <v>5.791476495678801</v>
+      </c>
+      <c r="AC290">
+        <v>0.7693716722165362</v>
+      </c>
+      <c r="AD290">
+        <v>0.3107615278267214</v>
+      </c>
+      <c r="AE290">
+        <v>321.7921253167856</v>
+      </c>
+      <c r="AF290">
+        <v>-274.0116480476877</v>
+      </c>
+      <c r="AG290">
+        <v>47.53254317180426</v>
+      </c>
+      <c r="AH290">
+        <v>20.33332794178119</v>
+      </c>
+      <c r="AI290">
+        <v>0.9135500332316681</v>
+      </c>
+      <c r="AJ290">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK290">
+        <v>0.002</v>
+      </c>
+      <c r="AL290">
+        <v>0.002</v>
+      </c>
+      <c r="AM290" s="2">
+        <v>37527</v>
+      </c>
+      <c r="AN290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:40">
+      <c r="A291" s="1">
+        <v>0</v>
+      </c>
+      <c r="B291" t="s">
+        <v>61</v>
+      </c>
+      <c r="C291">
+        <v>699</v>
+      </c>
+      <c r="D291">
+        <v>11</v>
+      </c>
+      <c r="E291">
+        <v>120.7205138344764</v>
+      </c>
+      <c r="F291">
+        <v>129.6169463683449</v>
+      </c>
+      <c r="G291">
+        <v>107.7050100947095</v>
+      </c>
+      <c r="H291">
+        <v>5.025500144416018</v>
+      </c>
+      <c r="I291">
+        <v>25.25565170152541</v>
+      </c>
+      <c r="J291">
+        <v>57.5049695259617</v>
+      </c>
+      <c r="K291">
+        <v>61.43634050995306</v>
+      </c>
+      <c r="L291">
+        <v>49.49438285616671</v>
+      </c>
+      <c r="M291">
+        <v>1.753861272163877</v>
+      </c>
+      <c r="N291">
+        <v>3.076029361996292</v>
+      </c>
+      <c r="O291">
+        <v>-0.03119963621040703</v>
+      </c>
+      <c r="P291">
+        <v>1.196434449531523</v>
+      </c>
+      <c r="Q291">
+        <v>-0.931743776211249</v>
+      </c>
+      <c r="R291">
+        <v>0.3644700805030502</v>
+      </c>
+      <c r="S291">
+        <v>0.1328384395818999</v>
+      </c>
+      <c r="T291">
+        <v>0.007238623143588817</v>
+      </c>
+      <c r="U291">
+        <v>1.384472473865763</v>
+      </c>
+      <c r="V291">
+        <v>-1.845544041308528</v>
+      </c>
+      <c r="W291">
+        <v>0.4217888438479315</v>
+      </c>
+      <c r="X291">
+        <v>0.1779058287945747</v>
+      </c>
+      <c r="Y291">
+        <v>58.03155460135935</v>
+      </c>
+      <c r="Z291">
+        <v>10.08209666247714</v>
+      </c>
+      <c r="AA291">
+        <v>14.22756830944768</v>
+      </c>
+      <c r="AB291">
+        <v>6.877157843179114</v>
+      </c>
+      <c r="AC291">
+        <v>0.7505450847993038</v>
+      </c>
+      <c r="AD291">
+        <v>0.5278104270597521</v>
+      </c>
+      <c r="AE291">
+        <v>333.664420951516</v>
+      </c>
+      <c r="AF291">
+        <v>-295.8881286283717</v>
+      </c>
+      <c r="AG291">
+        <v>45.53250713127206</v>
+      </c>
+      <c r="AH291">
+        <v>19.50986595519826</v>
+      </c>
+      <c r="AI291">
+        <v>0.9265592121292844</v>
+      </c>
+      <c r="AJ291">
+        <v>4.342371043379476</v>
+      </c>
+      <c r="AK291">
+        <v>0.002</v>
+      </c>
+      <c r="AL291">
+        <v>0.002</v>
+      </c>
+      <c r="AM291" s="2">
+        <v>37527</v>
+      </c>
+      <c r="AN291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:40">
+      <c r="A292" s="1">
+        <v>0</v>
+      </c>
+      <c r="B292" t="s">
+        <v>61</v>
+      </c>
+      <c r="C292">
+        <v>699</v>
+      </c>
+      <c r="D292">
+        <v>11</v>
+      </c>
+      <c r="E292">
+        <v>48.34305804625787</v>
+      </c>
+      <c r="F292">
+        <v>120.7882657782083</v>
+      </c>
+      <c r="G292">
+        <v>-2.916948782954616</v>
+      </c>
+      <c r="H292">
+        <v>46.13268529023917</v>
+      </c>
+      <c r="I292">
+        <v>2128.22465208825</v>
+      </c>
+      <c r="J292">
+        <v>23.56751600600805</v>
+      </c>
+      <c r="K292">
+        <v>62.73300451825486</v>
+      </c>
+      <c r="L292">
+        <v>-0.1634551481156307</v>
+      </c>
+      <c r="M292">
+        <v>26.14546844273259</v>
+      </c>
+      <c r="N292">
+        <v>683.5855200899259</v>
+      </c>
+      <c r="O292">
+        <v>-0.1945683975192194</v>
+      </c>
+      <c r="P292">
+        <v>1.461827934407204</v>
+      </c>
+      <c r="Q292">
+        <v>-2.60159773459219</v>
+      </c>
+      <c r="R292">
+        <v>0.6251249040152239</v>
+      </c>
+      <c r="S292">
+        <v>0.3907811456200429</v>
+      </c>
+      <c r="T292">
+        <v>-0.1226209940315991</v>
+      </c>
+      <c r="U292">
+        <v>1.107076448958736</v>
+      </c>
+      <c r="V292">
+        <v>-2.634171121067027</v>
+      </c>
+      <c r="W292">
+        <v>0.4415919328699502</v>
+      </c>
+      <c r="X292">
+        <v>0.1950034351758186</v>
+      </c>
+      <c r="Y292">
+        <v>11.99286228820528</v>
+      </c>
+      <c r="Z292">
+        <v>10.16288413711971</v>
+      </c>
+      <c r="AA292">
+        <v>14.72849279458017</v>
+      </c>
+      <c r="AB292">
+        <v>6.771624620428986</v>
+      </c>
+      <c r="AC292">
+        <v>0.7273886195757899</v>
+      </c>
+      <c r="AD292">
+        <v>0.2796996233255169</v>
+      </c>
+      <c r="AE292">
+        <v>338.4979239405656</v>
+      </c>
+      <c r="AF292">
+        <v>-332.627487410506</v>
+      </c>
+      <c r="AG292">
+        <v>53.95827607843128</v>
+      </c>
+      <c r="AH292">
+        <v>23.90493398935699</v>
+      </c>
+      <c r="AI292">
+        <v>-0.1110232653933913</v>
+      </c>
+      <c r="AJ292">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK292">
+        <v>0.002</v>
+      </c>
+      <c r="AL292">
+        <v>0.002</v>
+      </c>
+      <c r="AM292" s="2">
+        <v>37527</v>
+      </c>
+      <c r="AN292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:40">
+      <c r="A293" s="1">
+        <v>0</v>
+      </c>
+      <c r="B293" t="s">
+        <v>61</v>
+      </c>
+      <c r="C293">
+        <v>699</v>
+      </c>
+      <c r="D293">
+        <v>11</v>
+      </c>
+      <c r="E293">
+        <v>11.17037636519613</v>
+      </c>
+      <c r="F293">
+        <v>18.32465518607119</v>
+      </c>
+      <c r="G293">
+        <v>4.110504447787756</v>
+      </c>
+      <c r="H293">
+        <v>3.364645235421262</v>
+      </c>
+      <c r="I293">
+        <v>11.320837560243</v>
+      </c>
+      <c r="J293">
+        <v>1.186350417712222</v>
+      </c>
+      <c r="K293">
+        <v>2.126081819801854</v>
+      </c>
+      <c r="L293">
+        <v>0.0996064245252483</v>
+      </c>
+      <c r="M293">
+        <v>0.485409034931663</v>
+      </c>
+      <c r="N293">
+        <v>0.2356219311932884</v>
+      </c>
+      <c r="O293">
+        <v>-0.05372723315547259</v>
+      </c>
+      <c r="P293">
+        <v>2.028041690064633</v>
+      </c>
+      <c r="Q293">
+        <v>-1.818477652579947</v>
+      </c>
+      <c r="R293">
+        <v>0.5795093972583288</v>
+      </c>
+      <c r="S293">
+        <v>0.3358311415107116</v>
+      </c>
+      <c r="T293">
+        <v>0.0126020087133957</v>
+      </c>
+      <c r="U293">
+        <v>0.3765684736192298</v>
+      </c>
+      <c r="V293">
+        <v>-0.4209076638366867</v>
+      </c>
+      <c r="W293">
+        <v>0.129689702845125</v>
+      </c>
+      <c r="X293">
+        <v>0.01681941902405682</v>
+      </c>
+      <c r="Y293">
+        <v>1.393003228254403</v>
+      </c>
+      <c r="Z293">
+        <v>10.15544128136802</v>
+      </c>
+      <c r="AA293">
+        <v>11.10634503335818</v>
+      </c>
+      <c r="AB293">
+        <v>9.592398031774954</v>
+      </c>
+      <c r="AC293">
+        <v>0.1733909536513961</v>
+      </c>
+      <c r="AD293">
+        <v>0.3504298737445387</v>
+      </c>
+      <c r="AE293">
+        <v>104.7466054756205</v>
+      </c>
+      <c r="AF293">
+        <v>-64.43822270271883</v>
+      </c>
+      <c r="AG293">
+        <v>13.53761378668405</v>
+      </c>
+      <c r="AH293">
+        <v>5.396242805053659</v>
+      </c>
+      <c r="AI293">
+        <v>3.387232517068806</v>
+      </c>
+      <c r="AJ293">
+        <v>3.412122482104764</v>
+      </c>
+      <c r="AK293">
+        <v>0.009523809523809525</v>
+      </c>
+      <c r="AL293">
+        <v>0.009523809523809525</v>
+      </c>
+      <c r="AM293" s="2">
+        <v>37527</v>
+      </c>
+      <c r="AN293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:40">
+      <c r="A294" s="1">
+        <v>0</v>
+      </c>
+      <c r="B294" t="s">
+        <v>62</v>
+      </c>
+      <c r="C294">
+        <v>616</v>
+      </c>
+      <c r="D294">
+        <v>8</v>
+      </c>
+      <c r="E294">
+        <v>34.58280652999844</v>
+      </c>
+      <c r="F294">
+        <v>177.538801845468</v>
+      </c>
+      <c r="G294">
+        <v>-171.5189713012563</v>
+      </c>
+      <c r="H294">
+        <v>40.28196031736788</v>
+      </c>
+      <c r="I294">
+        <v>1622.636327010001</v>
+      </c>
+      <c r="J294">
+        <v>25.63082758264676</v>
+      </c>
+      <c r="K294">
+        <v>61.75438675201173</v>
+      </c>
+      <c r="L294">
+        <v>-1.45162910264132</v>
+      </c>
+      <c r="M294">
+        <v>23.69957603892492</v>
+      </c>
+      <c r="N294">
+        <v>561.6699044247845</v>
+      </c>
+      <c r="O294">
+        <v>0.1084058696019084</v>
+      </c>
+      <c r="P294">
+        <v>347.4039298010123</v>
+      </c>
+      <c r="Q294">
+        <v>-349.0577731467242</v>
+      </c>
+      <c r="R294">
+        <v>22.61690514213514</v>
+      </c>
+      <c r="S294">
+        <v>511.524398208339</v>
+      </c>
+      <c r="T294">
+        <v>0.1197203171934976</v>
+      </c>
+      <c r="U294">
+        <v>5.304644894779756</v>
+      </c>
+      <c r="V294">
+        <v>-1.530507253610083</v>
+      </c>
+      <c r="W294">
+        <v>0.633009708006472</v>
+      </c>
+      <c r="X294">
+        <v>0.400701290430439</v>
+      </c>
+      <c r="Y294">
+        <v>38.279136829704</v>
+      </c>
+      <c r="Z294">
+        <v>9.91917125958237</v>
+      </c>
+      <c r="AA294">
+        <v>16.19612608002296</v>
+      </c>
+      <c r="AB294">
+        <v>0</v>
+      </c>
+      <c r="AC294">
+        <v>1.168821805023817</v>
+      </c>
+      <c r="AD294">
+        <v>-0.3062190080175525</v>
+      </c>
+      <c r="AE294">
+        <v>477.9810197023675</v>
+      </c>
+      <c r="AF294">
+        <v>-386.7734876275592</v>
+      </c>
+      <c r="AG294">
+        <v>60.37211882018278</v>
+      </c>
+      <c r="AH294">
+        <v>23.06508758322494</v>
+      </c>
+      <c r="AI294">
+        <v>0.4392331302803817</v>
+      </c>
+      <c r="AJ294">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK294">
+        <v>0.002</v>
+      </c>
+      <c r="AL294">
+        <v>0.002</v>
+      </c>
+      <c r="AM294" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:40">
+      <c r="A295" s="1">
+        <v>0</v>
+      </c>
+      <c r="B295" t="s">
+        <v>62</v>
+      </c>
+      <c r="C295">
+        <v>616</v>
+      </c>
+      <c r="D295">
+        <v>8</v>
+      </c>
+      <c r="E295">
+        <v>55.2086465631116</v>
+      </c>
+      <c r="F295">
+        <v>65.61341119635527</v>
+      </c>
+      <c r="G295">
+        <v>45.67156578643132</v>
+      </c>
+      <c r="H295">
+        <v>3.052293373687561</v>
+      </c>
+      <c r="I295">
+        <v>9.316494839056993</v>
+      </c>
+      <c r="J295">
+        <v>59.98976550708903</v>
+      </c>
+      <c r="K295">
+        <v>62.49390479802642</v>
+      </c>
+      <c r="L295">
+        <v>55.25806392843592</v>
+      </c>
+      <c r="M295">
+        <v>1.363837097560413</v>
+      </c>
+      <c r="N295">
+        <v>1.86005162868201</v>
+      </c>
+      <c r="O295">
+        <v>0.0180054809570627</v>
+      </c>
+      <c r="P295">
+        <v>1.905891590472002</v>
+      </c>
+      <c r="Q295">
+        <v>-1.843669998721381</v>
+      </c>
+      <c r="R295">
+        <v>0.6548577668177414</v>
+      </c>
+      <c r="S295">
+        <v>0.4288386947615195</v>
+      </c>
+      <c r="T295">
+        <v>-0.002349736535346287</v>
+      </c>
+      <c r="U295">
+        <v>0.778847831472774</v>
+      </c>
+      <c r="V295">
+        <v>-0.8242013292552244</v>
+      </c>
+      <c r="W295">
+        <v>0.2757128240908612</v>
+      </c>
+      <c r="X295">
+        <v>0.07601756136815815</v>
+      </c>
+      <c r="Y295">
+        <v>60.55182247745024</v>
+      </c>
+      <c r="Z295">
+        <v>9.847869639452286</v>
+      </c>
+      <c r="AA295">
+        <v>11.99026271605422</v>
+      </c>
+      <c r="AB295">
+        <v>8.856551247522932</v>
+      </c>
+      <c r="AC295">
+        <v>0.3622402522562442</v>
+      </c>
+      <c r="AD295">
+        <v>0.2184264984200153</v>
+      </c>
+      <c r="AE295">
+        <v>124.6487236495414</v>
+      </c>
+      <c r="AF295">
+        <v>-234.9896326894643</v>
+      </c>
+      <c r="AG295">
+        <v>27.66350740905665</v>
+      </c>
+      <c r="AH295">
+        <v>14.97559875771912</v>
+      </c>
+      <c r="AI295">
+        <v>-1.636825999154492</v>
+      </c>
+      <c r="AJ295">
+        <v>4.342371043379476</v>
+      </c>
+      <c r="AK295">
+        <v>0.002</v>
+      </c>
+      <c r="AL295">
+        <v>0.002</v>
+      </c>
+      <c r="AM295" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:40">
+      <c r="A296" s="1">
+        <v>0</v>
+      </c>
+      <c r="B296" t="s">
+        <v>62</v>
+      </c>
+      <c r="C296">
+        <v>616</v>
+      </c>
+      <c r="D296">
+        <v>8</v>
+      </c>
+      <c r="E296">
+        <v>56.32332548175719</v>
+      </c>
+      <c r="F296">
+        <v>63.76689961995961</v>
+      </c>
+      <c r="G296">
+        <v>49.38069726997768</v>
+      </c>
+      <c r="H296">
+        <v>2.825398077205405</v>
+      </c>
+      <c r="I296">
+        <v>7.982874294676</v>
+      </c>
+      <c r="J296">
+        <v>58.94243049139239</v>
+      </c>
+      <c r="K296">
+        <v>62.26041350553442</v>
+      </c>
+      <c r="L296">
+        <v>52.23570306524684</v>
+      </c>
+      <c r="M296">
+        <v>2.086197682623248</v>
+      </c>
+      <c r="N296">
+        <v>4.352220770982608</v>
+      </c>
+      <c r="O296">
+        <v>-0.003144188042115946</v>
+      </c>
+      <c r="P296">
+        <v>1.615002074417639</v>
+      </c>
+      <c r="Q296">
+        <v>-1.762098643166141</v>
+      </c>
+      <c r="R296">
+        <v>0.6109644487331171</v>
+      </c>
+      <c r="S296">
+        <v>0.3732775576157616</v>
+      </c>
+      <c r="T296">
+        <v>-0.00298301411439867</v>
+      </c>
+      <c r="U296">
+        <v>0.7326565711671833</v>
+      </c>
+      <c r="V296">
+        <v>-0.9895012319281022</v>
+      </c>
+      <c r="W296">
+        <v>0.2583568309369879</v>
+      </c>
+      <c r="X296">
+        <v>0.06674825209180336</v>
+      </c>
+      <c r="Y296">
+        <v>59.8924097808883</v>
+      </c>
+      <c r="Z296">
+        <v>9.833295335522571</v>
+      </c>
+      <c r="AA296">
+        <v>10.73328933738395</v>
+      </c>
+      <c r="AB296">
+        <v>8.981809394548517</v>
+      </c>
+      <c r="AC296">
+        <v>0.2809867461165189</v>
+      </c>
+      <c r="AD296">
+        <v>0.2337796870352408</v>
+      </c>
+      <c r="AE296">
+        <v>115.7203603673662</v>
+      </c>
+      <c r="AF296">
+        <v>-145.1581655635969</v>
+      </c>
+      <c r="AG296">
+        <v>22.00905926690408</v>
+      </c>
+      <c r="AH296">
+        <v>12.61534494907954</v>
+      </c>
+      <c r="AI296">
+        <v>0.01208827254081393</v>
+      </c>
+      <c r="AJ296">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK296">
+        <v>0.002</v>
+      </c>
+      <c r="AL296">
+        <v>0.002</v>
+      </c>
+      <c r="AM296" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:40">
+      <c r="A297" s="1">
+        <v>0</v>
+      </c>
+      <c r="B297" t="s">
+        <v>62</v>
+      </c>
+      <c r="C297">
+        <v>616</v>
+      </c>
+      <c r="D297">
+        <v>8</v>
+      </c>
+      <c r="E297">
+        <v>59.10869013453446</v>
+      </c>
+      <c r="F297">
+        <v>65.96600292311314</v>
+      </c>
+      <c r="G297">
+        <v>53.44883137090974</v>
+      </c>
+      <c r="H297">
+        <v>2.708835040256078</v>
+      </c>
+      <c r="I297">
+        <v>7.337787275319149</v>
+      </c>
+      <c r="J297">
+        <v>60.50125216264554</v>
+      </c>
+      <c r="K297">
+        <v>63.76310124871151</v>
+      </c>
+      <c r="L297">
+        <v>55.08054112067791</v>
+      </c>
+      <c r="M297">
+        <v>1.37992682521497</v>
+      </c>
+      <c r="N297">
+        <v>1.904198042947866</v>
+      </c>
+      <c r="O297">
+        <v>0.009283289591371468</v>
+      </c>
+      <c r="P297">
+        <v>2.260060488723816</v>
+      </c>
+      <c r="Q297">
+        <v>-1.942963600426729</v>
+      </c>
+      <c r="R297">
+        <v>0.7246289664223994</v>
+      </c>
+      <c r="S297">
+        <v>0.5250871389783949</v>
+      </c>
+      <c r="T297">
+        <v>0.002039823704979689</v>
+      </c>
+      <c r="U297">
+        <v>1.112810616813533</v>
+      </c>
+      <c r="V297">
+        <v>-0.862215002768238</v>
+      </c>
+      <c r="W297">
+        <v>0.3142868256211078</v>
+      </c>
+      <c r="X297">
+        <v>0.09877620875899264</v>
+      </c>
+      <c r="Y297">
+        <v>60.85563880120566</v>
+      </c>
+      <c r="Z297">
+        <v>9.848658017618853</v>
+      </c>
+      <c r="AA297">
+        <v>11.45265471408267</v>
+      </c>
+      <c r="AB297">
+        <v>8.977822675905333</v>
+      </c>
+      <c r="AC297">
+        <v>0.3298366815030662</v>
+      </c>
+      <c r="AD297">
+        <v>0.1997105701323169</v>
+      </c>
+      <c r="AE297">
+        <v>106.9776238900308</v>
+      </c>
+      <c r="AF297">
+        <v>-135.9450462628279</v>
+      </c>
+      <c r="AG297">
+        <v>25.14488917207149</v>
+      </c>
+      <c r="AH297">
+        <v>14.8471028895081</v>
+      </c>
+      <c r="AI297">
+        <v>0.1021780015539011</v>
+      </c>
+      <c r="AJ297">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK297">
+        <v>0.002</v>
+      </c>
+      <c r="AL297">
+        <v>0.002</v>
+      </c>
+      <c r="AM297" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:40">
+      <c r="A298" s="1">
+        <v>0</v>
+      </c>
+      <c r="B298" t="s">
+        <v>62</v>
+      </c>
+      <c r="C298">
+        <v>616</v>
+      </c>
+      <c r="D298">
+        <v>8</v>
+      </c>
+      <c r="E298">
+        <v>11.21080195591072</v>
+      </c>
+      <c r="F298">
+        <v>63.81198190629721</v>
+      </c>
+      <c r="G298">
+        <v>-86.72464789762591</v>
+      </c>
+      <c r="H298">
+        <v>43.02376882295476</v>
+      </c>
+      <c r="I298">
+        <v>1851.044683731054</v>
+      </c>
+      <c r="J298">
+        <v>18.41448991875772</v>
+      </c>
+      <c r="K298">
+        <v>62.19968622124088</v>
+      </c>
+      <c r="L298">
+        <v>-2.823786827802252</v>
+      </c>
+      <c r="M298">
+        <v>22.84263300679886</v>
+      </c>
+      <c r="N298">
+        <v>521.7858826832966</v>
+      </c>
+      <c r="O298">
+        <v>-0.1840685706587881</v>
+      </c>
+      <c r="P298">
+        <v>4.369436246502216</v>
+      </c>
+      <c r="Q298">
+        <v>-6.726936337757462</v>
+      </c>
+      <c r="R298">
+        <v>1.456405983614811</v>
+      </c>
+      <c r="S298">
+        <v>2.121118389109025</v>
+      </c>
+      <c r="T298">
+        <v>-0.120987878797111</v>
+      </c>
+      <c r="U298">
+        <v>1.369377845764845</v>
+      </c>
+      <c r="V298">
+        <v>-2.604658963159224</v>
+      </c>
+      <c r="W298">
+        <v>0.4415314256469224</v>
+      </c>
+      <c r="X298">
+        <v>0.1949499998338038</v>
+      </c>
+      <c r="Y298">
+        <v>8.434475358843347</v>
+      </c>
+      <c r="Z298">
+        <v>9.90556398249065</v>
+      </c>
+      <c r="AA298">
+        <v>15.33045661420429</v>
+      </c>
+      <c r="AB298">
+        <v>5.281552801970269</v>
+      </c>
+      <c r="AC298">
+        <v>1.002211276962772</v>
+      </c>
+      <c r="AD298">
+        <v>-0.83794624115651</v>
+      </c>
+      <c r="AE298">
+        <v>496.9613413082106</v>
+      </c>
+      <c r="AF298">
+        <v>-394.8936747967819</v>
+      </c>
+      <c r="AG298">
+        <v>69.51386684640624</v>
+      </c>
+      <c r="AH298">
+        <v>29.60421176374842</v>
+      </c>
+      <c r="AI298">
+        <v>0.3043452118473827</v>
+      </c>
+      <c r="AJ298">
+        <v>4.354751391208961</v>
+      </c>
+      <c r="AK298">
+        <v>0.002</v>
+      </c>
+      <c r="AL298">
+        <v>0.002</v>
+      </c>
+      <c r="AM298" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:40">
+      <c r="A299" s="1">
+        <v>0</v>
+      </c>
+      <c r="B299" t="s">
+        <v>62</v>
+      </c>
+      <c r="C299">
+        <v>616</v>
+      </c>
+      <c r="D299">
+        <v>8</v>
+      </c>
+      <c r="E299">
+        <v>-29.65885743339944</v>
+      </c>
+      <c r="F299">
+        <v>-17.87397175518514</v>
+      </c>
+      <c r="G299">
+        <v>-52.28397594377788</v>
+      </c>
+      <c r="H299">
+        <v>9.722537723071905</v>
+      </c>
+      <c r="I299">
+        <v>94.52773977655623</v>
+      </c>
+      <c r="J299">
+        <v>-0.3110884489752823</v>
+      </c>
+      <c r="K299">
+        <v>0.9954149031563304</v>
+      </c>
+      <c r="L299">
+        <v>-2.113206297461389</v>
+      </c>
+      <c r="M299">
+        <v>0.7482645900862943</v>
+      </c>
+      <c r="N299">
+        <v>0.5598998967770101</v>
+      </c>
+      <c r="O299">
+        <v>-0.09479872723819763</v>
+      </c>
+      <c r="P299">
+        <v>1.204593633291175</v>
+      </c>
+      <c r="Q299">
+        <v>-1.520466021495501</v>
+      </c>
+      <c r="R299">
+        <v>0.5018302760010523</v>
+      </c>
+      <c r="S299">
+        <v>0.2518336259112923</v>
+      </c>
+      <c r="T299">
+        <v>-0.002337208671493812</v>
+      </c>
+      <c r="U299">
+        <v>0.5075066660026406</v>
+      </c>
+      <c r="V299">
+        <v>-0.5262003364593113</v>
+      </c>
+      <c r="W299">
+        <v>0.1221718901395024</v>
+      </c>
+      <c r="X299">
+        <v>0.01492597074025863</v>
+      </c>
+      <c r="Y299">
+        <v>-0.1026593130105481</v>
+      </c>
+      <c r="Z299">
+        <v>10.0395349570205</v>
+      </c>
+      <c r="AA299">
+        <v>10.54402200301194</v>
+      </c>
+      <c r="AB299">
+        <v>9.539538772917693</v>
+      </c>
+      <c r="AC299">
+        <v>0.08768009310517026</v>
+      </c>
+      <c r="AD299">
+        <v>-0.01692207952169849</v>
+      </c>
+      <c r="AE299">
+        <v>58.8567412332539</v>
+      </c>
+      <c r="AF299">
+        <v>-50.64052510069308</v>
+      </c>
+      <c r="AG299">
+        <v>7.605681168684167</v>
+      </c>
+      <c r="AH299">
+        <v>2.798061786097585</v>
+      </c>
+      <c r="AI299">
+        <v>0.8618822986837054</v>
+      </c>
+      <c r="AJ299">
+        <v>3.894063229815263</v>
+      </c>
+      <c r="AK299">
+        <v>0.003937007874015748</v>
+      </c>
+      <c r="AL299">
+        <v>0.003937007874015748</v>
+      </c>
+      <c r="AM299" s="2">
+        <v>35505</v>
+      </c>
+      <c r="AN299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:40">
+      <c r="A300" s="1">
+        <v>0</v>
+      </c>
+      <c r="B300" t="s">
+        <v>63</v>
+      </c>
+      <c r="C300">
+        <v>538</v>
+      </c>
+      <c r="D300">
+        <v>8</v>
+      </c>
+      <c r="E300">
+        <v>34.58280652999844</v>
+      </c>
+      <c r="F300">
+        <v>177.538801845468</v>
+      </c>
+      <c r="G300">
+        <v>-171.5189713012563</v>
+      </c>
+      <c r="H300">
+        <v>40.28196031736788</v>
+      </c>
+      <c r="I300">
+        <v>1622.636327010001</v>
+      </c>
+      <c r="J300">
+        <v>25.63082758264676</v>
+      </c>
+      <c r="K300">
+        <v>61.75438675201173</v>
+      </c>
+      <c r="L300">
+        <v>-1.45162910264132</v>
+      </c>
+      <c r="M300">
+        <v>23.69957603892492</v>
+      </c>
+      <c r="N300">
+        <v>561.6699044247845</v>
+      </c>
+      <c r="O300">
+        <v>0.1084058696019084</v>
+      </c>
+      <c r="P300">
+        <v>347.4039298010123</v>
+      </c>
+      <c r="Q300">
+        <v>-349.0577731467242</v>
+      </c>
+      <c r="R300">
+        <v>22.61690514213514</v>
+      </c>
+      <c r="S300">
+        <v>511.524398208339</v>
+      </c>
+      <c r="T300">
+        <v>0.1197203171934976</v>
+      </c>
+      <c r="U300">
+        <v>5.304644894779756</v>
+      </c>
+      <c r="V300">
+        <v>-1.530507253610083</v>
+      </c>
+      <c r="W300">
+        <v>0.633009708006472</v>
+      </c>
+      <c r="X300">
+        <v>0.400701290430439</v>
+      </c>
+      <c r="Y300">
+        <v>38.279136829704</v>
+      </c>
+      <c r="Z300">
+        <v>9.91917125958237</v>
+      </c>
+      <c r="AA300">
+        <v>16.19612608002296</v>
+      </c>
+      <c r="AB300">
+        <v>0</v>
+      </c>
+      <c r="AC300">
+        <v>1.168821805023817</v>
+      </c>
+      <c r="AD300">
+        <v>-0.3062190080175525</v>
+      </c>
+      <c r="AE300">
+        <v>477.9810197023675</v>
+      </c>
+      <c r="AF300">
+        <v>-386.7734876275592</v>
+      </c>
+      <c r="AG300">
+        <v>60.37211882018278</v>
+      </c>
+      <c r="AH300">
+        <v>23.06508758322494</v>
+      </c>
+      <c r="AI300">
+        <v>0.4392331302803817</v>
+      </c>
+      <c r="AJ300">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK300">
+        <v>0.002</v>
+      </c>
+      <c r="AL300">
+        <v>0.002</v>
+      </c>
+      <c r="AM300" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:40">
+      <c r="A301" s="1">
+        <v>0</v>
+      </c>
+      <c r="B301" t="s">
+        <v>63</v>
+      </c>
+      <c r="C301">
+        <v>538</v>
+      </c>
+      <c r="D301">
+        <v>8</v>
+      </c>
+      <c r="E301">
+        <v>55.2086465631116</v>
+      </c>
+      <c r="F301">
+        <v>65.61341119635527</v>
+      </c>
+      <c r="G301">
+        <v>45.67156578643132</v>
+      </c>
+      <c r="H301">
+        <v>3.052293373687561</v>
+      </c>
+      <c r="I301">
+        <v>9.316494839056993</v>
+      </c>
+      <c r="J301">
+        <v>59.98976550708903</v>
+      </c>
+      <c r="K301">
+        <v>62.49390479802642</v>
+      </c>
+      <c r="L301">
+        <v>55.25806392843592</v>
+      </c>
+      <c r="M301">
+        <v>1.363837097560413</v>
+      </c>
+      <c r="N301">
+        <v>1.86005162868201</v>
+      </c>
+      <c r="O301">
+        <v>0.0180054809570627</v>
+      </c>
+      <c r="P301">
+        <v>1.905891590472002</v>
+      </c>
+      <c r="Q301">
+        <v>-1.843669998721381</v>
+      </c>
+      <c r="R301">
+        <v>0.6548577668177414</v>
+      </c>
+      <c r="S301">
+        <v>0.4288386947615195</v>
+      </c>
+      <c r="T301">
+        <v>-0.002349736535346287</v>
+      </c>
+      <c r="U301">
+        <v>0.778847831472774</v>
+      </c>
+      <c r="V301">
+        <v>-0.8242013292552244</v>
+      </c>
+      <c r="W301">
+        <v>0.2757128240908612</v>
+      </c>
+      <c r="X301">
+        <v>0.07601756136815815</v>
+      </c>
+      <c r="Y301">
+        <v>60.55182247745024</v>
+      </c>
+      <c r="Z301">
+        <v>9.847869639452286</v>
+      </c>
+      <c r="AA301">
+        <v>11.99026271605422</v>
+      </c>
+      <c r="AB301">
+        <v>8.856551247522932</v>
+      </c>
+      <c r="AC301">
+        <v>0.3622402522562442</v>
+      </c>
+      <c r="AD301">
+        <v>0.2184264984200153</v>
+      </c>
+      <c r="AE301">
+        <v>124.6487236495414</v>
+      </c>
+      <c r="AF301">
+        <v>-234.9896326894643</v>
+      </c>
+      <c r="AG301">
+        <v>27.66350740905665</v>
+      </c>
+      <c r="AH301">
+        <v>14.97559875771912</v>
+      </c>
+      <c r="AI301">
+        <v>-1.636825999154492</v>
+      </c>
+      <c r="AJ301">
+        <v>4.342371043379476</v>
+      </c>
+      <c r="AK301">
+        <v>0.002</v>
+      </c>
+      <c r="AL301">
+        <v>0.002</v>
+      </c>
+      <c r="AM301" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:40">
+      <c r="A302" s="1">
+        <v>0</v>
+      </c>
+      <c r="B302" t="s">
+        <v>63</v>
+      </c>
+      <c r="C302">
+        <v>538</v>
+      </c>
+      <c r="D302">
+        <v>8</v>
+      </c>
+      <c r="E302">
+        <v>56.32332548175719</v>
+      </c>
+      <c r="F302">
+        <v>63.76689961995961</v>
+      </c>
+      <c r="G302">
+        <v>49.38069726997768</v>
+      </c>
+      <c r="H302">
+        <v>2.825398077205405</v>
+      </c>
+      <c r="I302">
+        <v>7.982874294676</v>
+      </c>
+      <c r="J302">
+        <v>58.94243049139239</v>
+      </c>
+      <c r="K302">
+        <v>62.26041350553442</v>
+      </c>
+      <c r="L302">
+        <v>52.23570306524684</v>
+      </c>
+      <c r="M302">
+        <v>2.086197682623248</v>
+      </c>
+      <c r="N302">
+        <v>4.352220770982608</v>
+      </c>
+      <c r="O302">
+        <v>-0.003144188042115946</v>
+      </c>
+      <c r="P302">
+        <v>1.615002074417639</v>
+      </c>
+      <c r="Q302">
+        <v>-1.762098643166141</v>
+      </c>
+      <c r="R302">
+        <v>0.6109644487331171</v>
+      </c>
+      <c r="S302">
+        <v>0.3732775576157616</v>
+      </c>
+      <c r="T302">
+        <v>-0.00298301411439867</v>
+      </c>
+      <c r="U302">
+        <v>0.7326565711671833</v>
+      </c>
+      <c r="V302">
+        <v>-0.9895012319281022</v>
+      </c>
+      <c r="W302">
+        <v>0.2583568309369879</v>
+      </c>
+      <c r="X302">
+        <v>0.06674825209180336</v>
+      </c>
+      <c r="Y302">
+        <v>59.8924097808883</v>
+      </c>
+      <c r="Z302">
+        <v>9.833295335522571</v>
+      </c>
+      <c r="AA302">
+        <v>10.73328933738395</v>
+      </c>
+      <c r="AB302">
+        <v>8.981809394548517</v>
+      </c>
+      <c r="AC302">
+        <v>0.2809867461165189</v>
+      </c>
+      <c r="AD302">
+        <v>0.2337796870352408</v>
+      </c>
+      <c r="AE302">
+        <v>115.7203603673662</v>
+      </c>
+      <c r="AF302">
+        <v>-145.1581655635969</v>
+      </c>
+      <c r="AG302">
+        <v>22.00905926690408</v>
+      </c>
+      <c r="AH302">
+        <v>12.61534494907954</v>
+      </c>
+      <c r="AI302">
+        <v>0.01208827254081393</v>
+      </c>
+      <c r="AJ302">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK302">
+        <v>0.002</v>
+      </c>
+      <c r="AL302">
+        <v>0.002</v>
+      </c>
+      <c r="AM302" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:40">
+      <c r="A303" s="1">
+        <v>0</v>
+      </c>
+      <c r="B303" t="s">
+        <v>63</v>
+      </c>
+      <c r="C303">
+        <v>538</v>
+      </c>
+      <c r="D303">
+        <v>8</v>
+      </c>
+      <c r="E303">
+        <v>59.10869013453446</v>
+      </c>
+      <c r="F303">
+        <v>65.96600292311314</v>
+      </c>
+      <c r="G303">
+        <v>53.44883137090974</v>
+      </c>
+      <c r="H303">
+        <v>2.708835040256078</v>
+      </c>
+      <c r="I303">
+        <v>7.337787275319149</v>
+      </c>
+      <c r="J303">
+        <v>60.50125216264554</v>
+      </c>
+      <c r="K303">
+        <v>63.76310124871151</v>
+      </c>
+      <c r="L303">
+        <v>55.08054112067791</v>
+      </c>
+      <c r="M303">
+        <v>1.37992682521497</v>
+      </c>
+      <c r="N303">
+        <v>1.904198042947866</v>
+      </c>
+      <c r="O303">
+        <v>0.009283289591371468</v>
+      </c>
+      <c r="P303">
+        <v>2.260060488723816</v>
+      </c>
+      <c r="Q303">
+        <v>-1.942963600426729</v>
+      </c>
+      <c r="R303">
+        <v>0.7246289664223994</v>
+      </c>
+      <c r="S303">
+        <v>0.5250871389783949</v>
+      </c>
+      <c r="T303">
+        <v>0.002039823704979689</v>
+      </c>
+      <c r="U303">
+        <v>1.112810616813533</v>
+      </c>
+      <c r="V303">
+        <v>-0.862215002768238</v>
+      </c>
+      <c r="W303">
+        <v>0.3142868256211078</v>
+      </c>
+      <c r="X303">
+        <v>0.09877620875899264</v>
+      </c>
+      <c r="Y303">
+        <v>60.85563880120566</v>
+      </c>
+      <c r="Z303">
+        <v>9.848658017618853</v>
+      </c>
+      <c r="AA303">
+        <v>11.45265471408267</v>
+      </c>
+      <c r="AB303">
+        <v>8.977822675905333</v>
+      </c>
+      <c r="AC303">
+        <v>0.3298366815030662</v>
+      </c>
+      <c r="AD303">
+        <v>0.1997105701323169</v>
+      </c>
+      <c r="AE303">
+        <v>106.9776238900308</v>
+      </c>
+      <c r="AF303">
+        <v>-135.9450462628279</v>
+      </c>
+      <c r="AG303">
+        <v>25.14488917207149</v>
+      </c>
+      <c r="AH303">
+        <v>14.8471028895081</v>
+      </c>
+      <c r="AI303">
+        <v>0.1021780015539011</v>
+      </c>
+      <c r="AJ303">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK303">
+        <v>0.002</v>
+      </c>
+      <c r="AL303">
+        <v>0.002</v>
+      </c>
+      <c r="AM303" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:40">
+      <c r="A304" s="1">
+        <v>0</v>
+      </c>
+      <c r="B304" t="s">
+        <v>63</v>
+      </c>
+      <c r="C304">
+        <v>538</v>
+      </c>
+      <c r="D304">
+        <v>8</v>
+      </c>
+      <c r="E304">
+        <v>11.21080195591072</v>
+      </c>
+      <c r="F304">
+        <v>63.81198190629721</v>
+      </c>
+      <c r="G304">
+        <v>-86.72464789762591</v>
+      </c>
+      <c r="H304">
+        <v>43.02376882295476</v>
+      </c>
+      <c r="I304">
+        <v>1851.044683731054</v>
+      </c>
+      <c r="J304">
+        <v>18.41448991875772</v>
+      </c>
+      <c r="K304">
+        <v>62.19968622124088</v>
+      </c>
+      <c r="L304">
+        <v>-2.823786827802252</v>
+      </c>
+      <c r="M304">
+        <v>22.84263300679886</v>
+      </c>
+      <c r="N304">
+        <v>521.7858826832966</v>
+      </c>
+      <c r="O304">
+        <v>-0.1840685706587881</v>
+      </c>
+      <c r="P304">
+        <v>4.369436246502216</v>
+      </c>
+      <c r="Q304">
+        <v>-6.726936337757462</v>
+      </c>
+      <c r="R304">
+        <v>1.456405983614811</v>
+      </c>
+      <c r="S304">
+        <v>2.121118389109025</v>
+      </c>
+      <c r="T304">
+        <v>-0.120987878797111</v>
+      </c>
+      <c r="U304">
+        <v>1.369377845764845</v>
+      </c>
+      <c r="V304">
+        <v>-2.604658963159224</v>
+      </c>
+      <c r="W304">
+        <v>0.4415314256469224</v>
+      </c>
+      <c r="X304">
+        <v>0.1949499998338038</v>
+      </c>
+      <c r="Y304">
+        <v>8.434475358843347</v>
+      </c>
+      <c r="Z304">
+        <v>9.90556398249065</v>
+      </c>
+      <c r="AA304">
+        <v>15.33045661420429</v>
+      </c>
+      <c r="AB304">
+        <v>5.281552801970269</v>
+      </c>
+      <c r="AC304">
+        <v>1.002211276962772</v>
+      </c>
+      <c r="AD304">
+        <v>-0.83794624115651</v>
+      </c>
+      <c r="AE304">
+        <v>496.9613413082106</v>
+      </c>
+      <c r="AF304">
+        <v>-394.8936747967819</v>
+      </c>
+      <c r="AG304">
+        <v>69.51386684640624</v>
+      </c>
+      <c r="AH304">
+        <v>29.60421176374842</v>
+      </c>
+      <c r="AI304">
+        <v>0.3043452118473827</v>
+      </c>
+      <c r="AJ304">
+        <v>4.354751391208961</v>
+      </c>
+      <c r="AK304">
+        <v>0.002</v>
+      </c>
+      <c r="AL304">
+        <v>0.002</v>
+      </c>
+      <c r="AM304" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:40">
+      <c r="A305" s="1">
+        <v>0</v>
+      </c>
+      <c r="B305" t="s">
+        <v>63</v>
+      </c>
+      <c r="C305">
+        <v>538</v>
+      </c>
+      <c r="D305">
+        <v>8</v>
+      </c>
+      <c r="E305">
+        <v>-29.65885743339944</v>
+      </c>
+      <c r="F305">
+        <v>-17.87397175518514</v>
+      </c>
+      <c r="G305">
+        <v>-52.28397594377788</v>
+      </c>
+      <c r="H305">
+        <v>9.722537723071905</v>
+      </c>
+      <c r="I305">
+        <v>94.52773977655623</v>
+      </c>
+      <c r="J305">
+        <v>-0.3110884489752823</v>
+      </c>
+      <c r="K305">
+        <v>0.9954149031563304</v>
+      </c>
+      <c r="L305">
+        <v>-2.113206297461389</v>
+      </c>
+      <c r="M305">
+        <v>0.7482645900862943</v>
+      </c>
+      <c r="N305">
+        <v>0.5598998967770101</v>
+      </c>
+      <c r="O305">
+        <v>-0.09479872723819763</v>
+      </c>
+      <c r="P305">
+        <v>1.204593633291175</v>
+      </c>
+      <c r="Q305">
+        <v>-1.520466021495501</v>
+      </c>
+      <c r="R305">
+        <v>0.5018302760010523</v>
+      </c>
+      <c r="S305">
+        <v>0.2518336259112923</v>
+      </c>
+      <c r="T305">
+        <v>-0.002337208671493812</v>
+      </c>
+      <c r="U305">
+        <v>0.5075066660026406</v>
+      </c>
+      <c r="V305">
+        <v>-0.5262003364593113</v>
+      </c>
+      <c r="W305">
+        <v>0.1221718901395024</v>
+      </c>
+      <c r="X305">
+        <v>0.01492597074025863</v>
+      </c>
+      <c r="Y305">
+        <v>-0.1026593130105481</v>
+      </c>
+      <c r="Z305">
+        <v>10.0395349570205</v>
+      </c>
+      <c r="AA305">
+        <v>10.54402200301194</v>
+      </c>
+      <c r="AB305">
+        <v>9.539538772917693</v>
+      </c>
+      <c r="AC305">
+        <v>0.08768009310517026</v>
+      </c>
+      <c r="AD305">
+        <v>-0.01692207952169849</v>
+      </c>
+      <c r="AE305">
+        <v>58.8567412332539</v>
+      </c>
+      <c r="AF305">
+        <v>-50.64052510069308</v>
+      </c>
+      <c r="AG305">
+        <v>7.605681168684167</v>
+      </c>
+      <c r="AH305">
+        <v>2.798061786097585</v>
+      </c>
+      <c r="AI305">
+        <v>0.8618822986837054</v>
+      </c>
+      <c r="AJ305">
+        <v>3.894063229815263</v>
+      </c>
+      <c r="AK305">
+        <v>0.003937007874015748</v>
+      </c>
+      <c r="AL305">
+        <v>0.003937007874015748</v>
+      </c>
+      <c r="AM305" s="2">
+        <v>37355</v>
+      </c>
+      <c r="AN305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:40">
+      <c r="A306" s="1">
+        <v>0</v>
+      </c>
+      <c r="B306" t="s">
+        <v>64</v>
+      </c>
+      <c r="C306">
+        <v>582</v>
+      </c>
+      <c r="D306">
+        <v>18</v>
+      </c>
+      <c r="E306">
+        <v>30.98156405248137</v>
+      </c>
+      <c r="F306">
+        <v>88.79324627265731</v>
+      </c>
+      <c r="G306">
+        <v>-2.918646367496668</v>
+      </c>
+      <c r="H306">
+        <v>24.33208700305265</v>
+      </c>
+      <c r="I306">
+        <v>592.0504579241237</v>
+      </c>
+      <c r="J306">
+        <v>28.53258439670157</v>
+      </c>
+      <c r="K306">
+        <v>57.50924873343547</v>
+      </c>
+      <c r="L306">
+        <v>-1.986662250492259</v>
+      </c>
+      <c r="M306">
+        <v>19.80347327438839</v>
+      </c>
+      <c r="N306">
+        <v>392.1775537294154</v>
+      </c>
+      <c r="O306">
+        <v>0.06725353052456778</v>
+      </c>
+      <c r="P306">
+        <v>9.78104502349607</v>
+      </c>
+      <c r="Q306">
+        <v>-9.064257082059775</v>
+      </c>
+      <c r="R306">
+        <v>1.498040466555166</v>
+      </c>
+      <c r="S306">
+        <v>2.24412523943682</v>
+      </c>
+      <c r="T306">
+        <v>0.1048413274226672</v>
+      </c>
+      <c r="U306">
+        <v>6.739754799304443</v>
+      </c>
+      <c r="V306">
+        <v>-3.67220922403294</v>
+      </c>
+      <c r="W306">
+        <v>1.091340368074164</v>
+      </c>
+      <c r="X306">
+        <v>1.191023798988251</v>
+      </c>
+      <c r="Y306">
+        <v>39.94204472849376</v>
+      </c>
+      <c r="Z306">
+        <v>10.5727233016945</v>
+      </c>
+      <c r="AA306">
+        <v>17.66903789118128</v>
+      </c>
+      <c r="AB306">
+        <v>0</v>
+      </c>
+      <c r="AC306">
+        <v>2.038179171337772</v>
+      </c>
+      <c r="AD306">
+        <v>0.8649998857553726</v>
+      </c>
+      <c r="AE306">
+        <v>656.3039039893001</v>
+      </c>
+      <c r="AF306">
+        <v>-679.4958751671838</v>
+      </c>
+      <c r="AG306">
+        <v>118.4470940323815</v>
+      </c>
+      <c r="AH306">
+        <v>59.49201698740706</v>
+      </c>
+      <c r="AI306">
+        <v>0.3926295662798328</v>
+      </c>
+      <c r="AJ306">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK306">
+        <v>0.002</v>
+      </c>
+      <c r="AL306">
+        <v>0.002</v>
+      </c>
+      <c r="AM306" s="2">
+        <v>37413</v>
+      </c>
+      <c r="AN306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:40">
+      <c r="A307" s="1">
+        <v>0</v>
+      </c>
+      <c r="B307" t="s">
+        <v>64</v>
+      </c>
+      <c r="C307">
+        <v>582</v>
+      </c>
+      <c r="D307">
+        <v>18</v>
+      </c>
+      <c r="E307">
+        <v>38.18632471102228</v>
+      </c>
+      <c r="F307">
+        <v>49.90818777257232</v>
+      </c>
+      <c r="G307">
+        <v>30.83662377090245</v>
+      </c>
+      <c r="H307">
+        <v>3.037045678186805</v>
+      </c>
+      <c r="I307">
+        <v>9.223646451393153</v>
+      </c>
+      <c r="J307">
+        <v>49.87067101531942</v>
+      </c>
+      <c r="K307">
+        <v>65.39024197300381</v>
+      </c>
+      <c r="L307">
+        <v>37.28884914146855</v>
+      </c>
+      <c r="M307">
+        <v>4.823435723260584</v>
+      </c>
+      <c r="N307">
+        <v>23.26553217642635</v>
+      </c>
+      <c r="O307">
+        <v>0.03210063942314424</v>
+      </c>
+      <c r="P307">
+        <v>2.408201709619114</v>
+      </c>
+      <c r="Q307">
+        <v>-2.852531329602844</v>
+      </c>
+      <c r="R307">
+        <v>0.6180530756159999</v>
+      </c>
+      <c r="S307">
+        <v>0.3819896042783968</v>
+      </c>
+      <c r="T307">
+        <v>-0.01453150861007401</v>
+      </c>
+      <c r="U307">
+        <v>3.074905864368873</v>
+      </c>
+      <c r="V307">
+        <v>-3.592748612952732</v>
+      </c>
+      <c r="W307">
+        <v>1.097351857502532</v>
+      </c>
+      <c r="X307">
+        <v>1.204181099164257</v>
+      </c>
+      <c r="Y307">
+        <v>50.51460694422467</v>
+      </c>
+      <c r="Z307">
+        <v>10.68766488640907</v>
+      </c>
+      <c r="AA307">
+        <v>21.66916242036134</v>
+      </c>
+      <c r="AB307">
+        <v>5.413372331550824</v>
+      </c>
+      <c r="AC307">
+        <v>2.18127908179669</v>
+      </c>
+      <c r="AD307">
+        <v>0.08634917393325701</v>
+      </c>
+      <c r="AE307">
+        <v>785.1040260196903</v>
+      </c>
+      <c r="AF307">
+        <v>-1174.351427132222</v>
+      </c>
+      <c r="AG307">
+        <v>138.9523808698717</v>
+      </c>
+      <c r="AH307">
+        <v>74.03100090916718</v>
+      </c>
+      <c r="AI307">
+        <v>-1.12036675211516</v>
+      </c>
+      <c r="AJ307">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK307">
+        <v>0.002</v>
+      </c>
+      <c r="AL307">
+        <v>0.002</v>
+      </c>
+      <c r="AM307" s="2">
+        <v>37413</v>
+      </c>
+      <c r="AN307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:40">
+      <c r="A308" s="1">
+        <v>0</v>
+      </c>
+      <c r="B308" t="s">
+        <v>64</v>
+      </c>
+      <c r="C308">
+        <v>582</v>
+      </c>
+      <c r="D308">
+        <v>18</v>
+      </c>
+      <c r="E308">
+        <v>47.1531374740295</v>
+      </c>
+      <c r="F308">
+        <v>69.80183484735142</v>
+      </c>
+      <c r="G308">
+        <v>28.5737534373223</v>
+      </c>
+      <c r="H308">
+        <v>7.871672812528382</v>
+      </c>
+      <c r="I308">
+        <v>61.96323286749848</v>
+      </c>
+      <c r="J308">
+        <v>49.39016009348094</v>
+      </c>
+      <c r="K308">
+        <v>61.82607971946857</v>
+      </c>
+      <c r="L308">
+        <v>32.49854542133605</v>
+      </c>
+      <c r="M308">
+        <v>5.266620421223561</v>
+      </c>
+      <c r="N308">
+        <v>27.73729066124905</v>
+      </c>
+      <c r="O308">
+        <v>0.02826762327864049</v>
+      </c>
+      <c r="P308">
+        <v>2.672290686598686</v>
+      </c>
+      <c r="Q308">
+        <v>-3.099456543477967</v>
+      </c>
+      <c r="R308">
+        <v>0.6622422057896102</v>
+      </c>
+      <c r="S308">
+        <v>0.4385647391290885</v>
+      </c>
+      <c r="T308">
+        <v>0.004340712427588067</v>
+      </c>
+      <c r="U308">
+        <v>2.925685534793956</v>
+      </c>
+      <c r="V308">
+        <v>-3.325978686001939</v>
+      </c>
+      <c r="W308">
+        <v>0.9040037138929874</v>
+      </c>
+      <c r="X308">
+        <v>0.8172227147323141</v>
+      </c>
+      <c r="Y308">
+        <v>50.60727508275838</v>
+      </c>
+      <c r="Z308">
+        <v>10.43594235063467</v>
+      </c>
+      <c r="AA308">
+        <v>22.24360807063458</v>
+      </c>
+      <c r="AB308">
+        <v>4.655684697227681</v>
+      </c>
+      <c r="AC308">
+        <v>1.861818194187121</v>
+      </c>
+      <c r="AD308">
+        <v>0.2505712000494683</v>
+      </c>
+      <c r="AE308">
+        <v>836.8681062499079</v>
+      </c>
+      <c r="AF308">
+        <v>-675.5043965408186</v>
+      </c>
+      <c r="AG308">
+        <v>114.4573161578445</v>
+      </c>
+      <c r="AH308">
+        <v>57.72432907000898</v>
+      </c>
+      <c r="AI308">
+        <v>0.07417179167846132</v>
+      </c>
+      <c r="AJ308">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK308">
+        <v>0.002</v>
+      </c>
+      <c r="AL308">
+        <v>0.002</v>
+      </c>
+      <c r="AM308" s="2">
+        <v>37413</v>
+      </c>
+      <c r="AN308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:40">
+      <c r="A309" s="1">
+        <v>0</v>
+      </c>
+      <c r="B309" t="s">
+        <v>64</v>
+      </c>
+      <c r="C309">
+        <v>582</v>
+      </c>
+      <c r="D309">
+        <v>18</v>
+      </c>
+      <c r="E309">
+        <v>15.12387928150039</v>
+      </c>
+      <c r="F309">
+        <v>63.70784503463805</v>
+      </c>
+      <c r="G309">
+        <v>-6.560555933735392</v>
+      </c>
+      <c r="H309">
+        <v>24.97711654581159</v>
+      </c>
+      <c r="I309">
+        <v>623.856350943055</v>
+      </c>
+      <c r="J309">
+        <v>23.27827499774821</v>
+      </c>
+      <c r="K309">
+        <v>63.41455069951309</v>
+      </c>
+      <c r="L309">
+        <v>2.670826271398013</v>
+      </c>
+      <c r="M309">
+        <v>22.13200239868187</v>
+      </c>
+      <c r="N309">
+        <v>489.8255301752599</v>
+      </c>
+      <c r="O309">
+        <v>-0.1380246489313085</v>
+      </c>
+      <c r="P309">
+        <v>1.395547948637549</v>
+      </c>
+      <c r="Q309">
+        <v>-1.958577846672664</v>
+      </c>
+      <c r="R309">
+        <v>0.4050099732313086</v>
+      </c>
+      <c r="S309">
+        <v>0.1640330784168253</v>
+      </c>
+      <c r="T309">
+        <v>-0.08384879529481677</v>
+      </c>
+      <c r="U309">
+        <v>1.826014974857344</v>
+      </c>
+      <c r="V309">
+        <v>-3.041402869022562</v>
+      </c>
+      <c r="W309">
+        <v>0.583686216868012</v>
+      </c>
+      <c r="X309">
+        <v>0.340689599761692</v>
+      </c>
+      <c r="Y309">
+        <v>21.0046399546954</v>
+      </c>
+      <c r="Z309">
+        <v>10.17719933509533</v>
+      </c>
+      <c r="AA309">
+        <v>18.65902998550568</v>
+      </c>
+      <c r="AB309">
+        <v>6.676331327907565</v>
+      </c>
+      <c r="AC309">
+        <v>1.287420831947299</v>
+      </c>
+      <c r="AD309">
+        <v>-0.9114010107905817</v>
+      </c>
+      <c r="AE309">
+        <v>504.4615932022441</v>
+      </c>
+      <c r="AF309">
+        <v>-452.3709743552325</v>
+      </c>
+      <c r="AG309">
+        <v>67.72921674219924</v>
+      </c>
+      <c r="AH309">
+        <v>28.41004978745485</v>
+      </c>
+      <c r="AI309">
+        <v>0.3671070385098542</v>
+      </c>
+      <c r="AJ309">
+        <v>4.267857747078641</v>
+      </c>
+      <c r="AK309">
+        <v>0.002</v>
+      </c>
+      <c r="AL309">
+        <v>0.002</v>
+      </c>
+      <c r="AM309" s="2">
+        <v>37413</v>
+      </c>
+      <c r="AN309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:40">
+      <c r="A310" s="1">
+        <v>0</v>
+      </c>
+      <c r="B310" t="s">
+        <v>64</v>
+      </c>
+      <c r="C310">
+        <v>582</v>
+      </c>
+      <c r="D310">
+        <v>18</v>
+      </c>
+      <c r="E310">
+        <v>0.3158957640094493</v>
+      </c>
+      <c r="F310">
+        <v>2.24964955360769</v>
+      </c>
+      <c r="G310">
+        <v>-4.721980748772396</v>
+      </c>
+      <c r="H310">
+        <v>1.964941520378586</v>
+      </c>
+      <c r="I310">
+        <v>3.860995178507708</v>
+      </c>
+      <c r="J310">
+        <v>1.433193850244976</v>
+      </c>
+      <c r="K310">
+        <v>4.106075982355009</v>
+      </c>
+      <c r="L310">
+        <v>0.498659694238782</v>
+      </c>
+      <c r="M310">
+        <v>0.9562766116783168</v>
+      </c>
+      <c r="N310">
+        <v>0.9144649580429622</v>
+      </c>
+      <c r="O310">
+        <v>0.1220533241979386</v>
+      </c>
+      <c r="P310">
+        <v>0.4890559940398214</v>
+      </c>
+      <c r="Q310">
+        <v>-0.2875727158936487</v>
+      </c>
+      <c r="R310">
+        <v>0.1676354525180145</v>
+      </c>
+      <c r="S310">
+        <v>0.0281016449409195</v>
+      </c>
+      <c r="T310">
+        <v>-0.06079033987647278</v>
+      </c>
+      <c r="U310">
+        <v>0.4186767565290666</v>
+      </c>
+      <c r="V310">
+        <v>-0.2997589036364445</v>
+      </c>
+      <c r="W310">
+        <v>0.133193030412136</v>
+      </c>
+      <c r="X310">
+        <v>0.01774038335036818</v>
+      </c>
+      <c r="Y310">
+        <v>1.079917191309056</v>
+      </c>
+      <c r="Z310">
+        <v>10.2016929500472</v>
+      </c>
+      <c r="AA310">
+        <v>11.18837789851594</v>
+      </c>
+      <c r="AB310">
+        <v>9.747671516829032</v>
+      </c>
+      <c r="AC310">
+        <v>0.2274965369150539</v>
+      </c>
+      <c r="AD310">
+        <v>-1.123448509980748</v>
+      </c>
+      <c r="AE310">
+        <v>74.28759771213977</v>
+      </c>
+      <c r="AF310">
+        <v>-111.4164403843723</v>
+      </c>
+      <c r="AG310">
+        <v>24.43529358838373</v>
+      </c>
+      <c r="AH310">
+        <v>11.93884075468099</v>
+      </c>
+      <c r="AI310">
+        <v>-0.9356233576359322</v>
+      </c>
+      <c r="AJ310">
+        <v>2.89277064282884</v>
+      </c>
+      <c r="AK310">
+        <v>0.01818181818181818</v>
+      </c>
+      <c r="AL310">
+        <v>0.01818181818181818</v>
+      </c>
+      <c r="AM310" s="2">
+        <v>37413</v>
+      </c>
+      <c r="AN310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:40">
+      <c r="A311" s="1">
+        <v>0</v>
+      </c>
+      <c r="B311" t="s">
+        <v>65</v>
+      </c>
+      <c r="C311">
+        <v>699</v>
+      </c>
+      <c r="D311">
+        <v>9</v>
+      </c>
+      <c r="E311">
+        <v>48.5228745686976</v>
+      </c>
+      <c r="F311">
+        <v>135.3005581327055</v>
+      </c>
+      <c r="G311">
+        <v>-6.54836847835009</v>
+      </c>
+      <c r="H311">
+        <v>57.68856801801901</v>
+      </c>
+      <c r="I311">
+        <v>3327.970879969605</v>
+      </c>
+      <c r="J311">
+        <v>13.20091920754935</v>
+      </c>
+      <c r="K311">
+        <v>51.72820652454038</v>
+      </c>
+      <c r="L311">
+        <v>0.2319462741084379</v>
+      </c>
+      <c r="M311">
+        <v>16.64836308509385</v>
+      </c>
+      <c r="N311">
+        <v>277.1679934131156</v>
+      </c>
+      <c r="O311">
+        <v>0.2514124979886188</v>
+      </c>
+      <c r="P311">
+        <v>9.197161783475906</v>
+      </c>
+      <c r="Q311">
+        <v>-7.632483863414734</v>
+      </c>
+      <c r="R311">
+        <v>1.724806981904136</v>
+      </c>
+      <c r="S311">
+        <v>2.974959124825253</v>
+      </c>
+      <c r="T311">
+        <v>0.0978894847960694</v>
+      </c>
+      <c r="U311">
+        <v>2.261572406513146</v>
+      </c>
+      <c r="V311">
+        <v>-1.136497656323428</v>
+      </c>
+      <c r="W311">
+        <v>0.4024346290952662</v>
+      </c>
+      <c r="X311">
+        <v>0.1619536306950445</v>
+      </c>
+      <c r="Y311">
+        <v>7.141663131685786</v>
+      </c>
+      <c r="Z311">
+        <v>10.14197917867316</v>
+      </c>
+      <c r="AA311">
+        <v>13.8616701735397</v>
+      </c>
+      <c r="AB311">
+        <v>0</v>
+      </c>
+      <c r="AC311">
+        <v>0.8615937714572665</v>
+      </c>
+      <c r="AD311">
+        <v>0.02941088997286756</v>
+      </c>
+      <c r="AE311">
+        <v>443.6115130237329</v>
+      </c>
+      <c r="AF311">
+        <v>-440.3862776268343</v>
+      </c>
+      <c r="AG311">
+        <v>57.86769954062205</v>
+      </c>
+      <c r="AH311">
+        <v>23.3083372287096</v>
+      </c>
+      <c r="AI311">
+        <v>-0.165431131038938</v>
+      </c>
+      <c r="AJ311">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK311">
+        <v>0.002</v>
+      </c>
+      <c r="AL311">
+        <v>0.002</v>
+      </c>
+      <c r="AM311" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:40">
+      <c r="A312" s="1">
+        <v>0</v>
+      </c>
+      <c r="B312" t="s">
+        <v>65</v>
+      </c>
+      <c r="C312">
+        <v>699</v>
+      </c>
+      <c r="D312">
+        <v>9</v>
+      </c>
+      <c r="E312">
+        <v>120.3330456163294</v>
+      </c>
+      <c r="F312">
+        <v>127.7468106146803</v>
+      </c>
+      <c r="G312">
+        <v>112.8826048288062</v>
+      </c>
+      <c r="H312">
+        <v>3.476930124245065</v>
+      </c>
+      <c r="I312">
+        <v>12.0890430888828</v>
+      </c>
+      <c r="J312">
+        <v>53.4370778683443</v>
+      </c>
+      <c r="K312">
+        <v>58.00589251656402</v>
+      </c>
+      <c r="L312">
+        <v>47.7712031795827</v>
+      </c>
+      <c r="M312">
+        <v>1.744799152544285</v>
+      </c>
+      <c r="N312">
+        <v>3.044324082719256</v>
+      </c>
+      <c r="O312">
+        <v>-0.01913488063183552</v>
+      </c>
+      <c r="P312">
+        <v>1.228689703891405</v>
+      </c>
+      <c r="Q312">
+        <v>-1.290607133241366</v>
+      </c>
+      <c r="R312">
+        <v>0.3673058511538359</v>
+      </c>
+      <c r="S312">
+        <v>0.1349135882918439</v>
+      </c>
+      <c r="T312">
+        <v>0.008831281139806722</v>
+      </c>
+      <c r="U312">
+        <v>1.048391288705574</v>
+      </c>
+      <c r="V312">
+        <v>-1.124413939017394</v>
+      </c>
+      <c r="W312">
+        <v>0.2748395469957342</v>
+      </c>
+      <c r="X312">
+        <v>0.07553677659282035</v>
+      </c>
+      <c r="Y312">
+        <v>54.05660432535034</v>
+      </c>
+      <c r="Z312">
+        <v>10.03555170008285</v>
+      </c>
+      <c r="AA312">
+        <v>13.02721382337758</v>
+      </c>
+      <c r="AB312">
+        <v>6.374527433465167</v>
+      </c>
+      <c r="AC312">
+        <v>0.7208965658687407</v>
+      </c>
+      <c r="AD312">
+        <v>-0.3410956056869444</v>
+      </c>
+      <c r="AE312">
+        <v>316.1835593645075</v>
+      </c>
+      <c r="AF312">
+        <v>-167.8383376601892</v>
+      </c>
+      <c r="AG312">
+        <v>39.58768519594553</v>
+      </c>
+      <c r="AH312">
+        <v>19.43919267121569</v>
+      </c>
+      <c r="AI312">
+        <v>1.200172594334693</v>
+      </c>
+      <c r="AJ312">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK312">
+        <v>0.002</v>
+      </c>
+      <c r="AL312">
+        <v>0.002</v>
+      </c>
+      <c r="AM312" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:40">
+      <c r="A313" s="1">
+        <v>0</v>
+      </c>
+      <c r="B313" t="s">
+        <v>65</v>
+      </c>
+      <c r="C313">
+        <v>699</v>
+      </c>
+      <c r="D313">
+        <v>9</v>
+      </c>
+      <c r="E313">
+        <v>120.982665013047</v>
+      </c>
+      <c r="F313">
+        <v>129.9920584466862</v>
+      </c>
+      <c r="G313">
+        <v>113.0052783475256</v>
+      </c>
+      <c r="H313">
+        <v>3.138213077067307</v>
+      </c>
+      <c r="I313">
+        <v>9.848381317076253</v>
+      </c>
+      <c r="J313">
+        <v>56.01175273635929</v>
+      </c>
+      <c r="K313">
+        <v>60.93192248645977</v>
+      </c>
+      <c r="L313">
+        <v>51.42649608813957</v>
+      </c>
+      <c r="M313">
+        <v>1.948210408551389</v>
+      </c>
+      <c r="N313">
+        <v>3.795523795987969</v>
+      </c>
+      <c r="O313">
+        <v>0.02285785060667523</v>
+      </c>
+      <c r="P313">
+        <v>1.479027764562275</v>
+      </c>
+      <c r="Q313">
+        <v>-1.252605537325394</v>
+      </c>
+      <c r="R313">
+        <v>0.4201944977861297</v>
+      </c>
+      <c r="S313">
+        <v>0.1765634159697378</v>
+      </c>
+      <c r="T313">
+        <v>0.000336654738320051</v>
+      </c>
+      <c r="U313">
+        <v>1.04626635878364</v>
+      </c>
+      <c r="V313">
+        <v>-1.072089530665011</v>
+      </c>
+      <c r="W313">
+        <v>0.3644865407861154</v>
+      </c>
+      <c r="X313">
+        <v>0.1328504384142286</v>
+      </c>
+      <c r="Y313">
+        <v>56.49585790733138</v>
+      </c>
+      <c r="Z313">
+        <v>10.07387612978396</v>
+      </c>
+      <c r="AA313">
+        <v>13.6348010619884</v>
+      </c>
+      <c r="AB313">
+        <v>7.278756761975221</v>
+      </c>
+      <c r="AC313">
+        <v>0.7217267493798559</v>
+      </c>
+      <c r="AD313">
+        <v>-0.3087060612280991</v>
+      </c>
+      <c r="AE313">
+        <v>370.6908717049055</v>
+      </c>
+      <c r="AF313">
+        <v>-285.5400771618649</v>
+      </c>
+      <c r="AG313">
+        <v>48.14036551109306</v>
+      </c>
+      <c r="AH313">
+        <v>24.86332685556534</v>
+      </c>
+      <c r="AI313">
+        <v>0.502009301737625</v>
+      </c>
+      <c r="AJ313">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK313">
+        <v>0.002</v>
+      </c>
+      <c r="AL313">
+        <v>0.002</v>
+      </c>
+      <c r="AM313" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:40">
+      <c r="A314" s="1">
+        <v>0</v>
+      </c>
+      <c r="B314" t="s">
+        <v>65</v>
+      </c>
+      <c r="C314">
+        <v>699</v>
+      </c>
+      <c r="D314">
+        <v>9</v>
+      </c>
+      <c r="E314">
+        <v>116.2144649699363</v>
+      </c>
+      <c r="F314">
+        <v>128.3979466575708</v>
+      </c>
+      <c r="G314">
+        <v>107.4499608345613</v>
+      </c>
+      <c r="H314">
+        <v>4.971284122697254</v>
+      </c>
+      <c r="I314">
+        <v>24.71366582858181</v>
+      </c>
+      <c r="J314">
+        <v>58.56407770024167</v>
+      </c>
+      <c r="K314">
+        <v>65.04977939745029</v>
+      </c>
+      <c r="L314">
+        <v>51.04874497555949</v>
+      </c>
+      <c r="M314">
+        <v>3.183547436956777</v>
+      </c>
+      <c r="N314">
+        <v>10.13497428335406</v>
+      </c>
+      <c r="O314">
+        <v>-0.03876141354030341</v>
+      </c>
+      <c r="P314">
+        <v>1.707045764961279</v>
+      </c>
+      <c r="Q314">
+        <v>-1.704614434965421</v>
+      </c>
+      <c r="R314">
+        <v>0.5048704644443154</v>
+      </c>
+      <c r="S314">
+        <v>0.2548941858682187</v>
+      </c>
+      <c r="T314">
+        <v>0.01265182759020351</v>
+      </c>
+      <c r="U314">
+        <v>1.294101958145944</v>
+      </c>
+      <c r="V314">
+        <v>-1.600708630238955</v>
+      </c>
+      <c r="W314">
+        <v>0.3508836323056759</v>
+      </c>
+      <c r="X314">
+        <v>0.1231193234200247</v>
+      </c>
+      <c r="Y314">
+        <v>59.82745567487738</v>
+      </c>
+      <c r="Z314">
+        <v>10.10317675016816</v>
+      </c>
+      <c r="AA314">
+        <v>14.11732977584642</v>
+      </c>
+      <c r="AB314">
+        <v>5.95353676397484</v>
+      </c>
+      <c r="AC314">
+        <v>0.9209118917064192</v>
+      </c>
+      <c r="AD314">
+        <v>0.2066493322552044</v>
+      </c>
+      <c r="AE314">
+        <v>340.9452950057301</v>
+      </c>
+      <c r="AF314">
+        <v>-249.1614548285767</v>
+      </c>
+      <c r="AG314">
+        <v>52.31057601887992</v>
+      </c>
+      <c r="AH314">
+        <v>27.04694274080115</v>
+      </c>
+      <c r="AI314">
+        <v>0.1906158181631388</v>
+      </c>
+      <c r="AJ314">
+        <v>4.342371043379476</v>
+      </c>
+      <c r="AK314">
+        <v>0.002</v>
+      </c>
+      <c r="AL314">
+        <v>0.002</v>
+      </c>
+      <c r="AM314" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:40">
+      <c r="A315" s="1">
+        <v>0</v>
+      </c>
+      <c r="B315" t="s">
+        <v>65</v>
+      </c>
+      <c r="C315">
+        <v>699</v>
+      </c>
+      <c r="D315">
+        <v>9</v>
+      </c>
+      <c r="E315">
+        <v>88.73807357070901</v>
+      </c>
+      <c r="F315">
+        <v>174.6382052355972</v>
+      </c>
+      <c r="G315">
+        <v>-178.6058107874144</v>
+      </c>
+      <c r="H315">
+        <v>40.96445468814657</v>
+      </c>
+      <c r="I315">
+        <v>1678.086547897213</v>
+      </c>
+      <c r="J315">
+        <v>50.7536187460854</v>
+      </c>
+      <c r="K315">
+        <v>85.51771371951071</v>
+      </c>
+      <c r="L315">
+        <v>8.604584484404711</v>
+      </c>
+      <c r="M315">
+        <v>15.7646862326814</v>
+      </c>
+      <c r="N315">
+        <v>248.5253320148943</v>
+      </c>
+      <c r="O315">
+        <v>-0.2417121876851939</v>
+      </c>
+      <c r="P315">
+        <v>346.8988377196234</v>
+      </c>
+      <c r="Q315">
+        <v>-353.2440160230116</v>
+      </c>
+      <c r="R315">
+        <v>22.2764026998814</v>
+      </c>
+      <c r="S315">
+        <v>496.2381172472832</v>
+      </c>
+      <c r="T315">
+        <v>-0.1094925041854202</v>
+      </c>
+      <c r="U315">
+        <v>2.786116997526165</v>
+      </c>
+      <c r="V315">
+        <v>-2.691470561376036</v>
+      </c>
+      <c r="W315">
+        <v>0.6075906210921189</v>
+      </c>
+      <c r="X315">
+        <v>0.3691663628391069</v>
+      </c>
+      <c r="Y315">
+        <v>58.13859967181333</v>
+      </c>
+      <c r="Z315">
+        <v>10.16001876820288</v>
+      </c>
+      <c r="AA315">
+        <v>16.61058096515591</v>
+      </c>
+      <c r="AB315">
+        <v>6.566772418776214</v>
+      </c>
+      <c r="AC315">
+        <v>0.9856470107623295</v>
+      </c>
+      <c r="AD315">
+        <v>0.1117222715256055</v>
+      </c>
+      <c r="AE315">
+        <v>314.9488221671266</v>
+      </c>
+      <c r="AF315">
+        <v>-551.8285378482082</v>
+      </c>
+      <c r="AG315">
+        <v>60.49867978574379</v>
+      </c>
+      <c r="AH315">
+        <v>27.20377542425647</v>
+      </c>
+      <c r="AI315">
+        <v>-2.590360795117307</v>
+      </c>
+      <c r="AJ315">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK315">
+        <v>0.002</v>
+      </c>
+      <c r="AL315">
+        <v>0.002</v>
+      </c>
+      <c r="AM315" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:40">
+      <c r="A316" s="1">
+        <v>0</v>
+      </c>
+      <c r="B316" t="s">
+        <v>65</v>
+      </c>
+      <c r="C316">
+        <v>699</v>
+      </c>
+      <c r="D316">
+        <v>9</v>
+      </c>
+      <c r="E316">
+        <v>-9.244423532928911</v>
+      </c>
+      <c r="F316">
+        <v>-3.683017093161012</v>
+      </c>
+      <c r="G316">
+        <v>-14.83555198945786</v>
+      </c>
+      <c r="H316">
+        <v>4.071185398412943</v>
+      </c>
+      <c r="I316">
+        <v>16.57455054825076</v>
+      </c>
+      <c r="J316">
+        <v>5.966207903978481</v>
+      </c>
+      <c r="K316">
+        <v>9.993660769963329</v>
+      </c>
+      <c r="L316">
+        <v>2.531121986993455</v>
+      </c>
+      <c r="M316">
+        <v>2.314072827671185</v>
+      </c>
+      <c r="N316">
+        <v>5.354933051766114</v>
+      </c>
+      <c r="O316">
+        <v>-0.004494971874393772</v>
+      </c>
+      <c r="P316">
+        <v>0.8564624853202822</v>
+      </c>
+      <c r="Q316">
+        <v>-0.7596969783283383</v>
+      </c>
+      <c r="R316">
+        <v>0.3030660443752328</v>
+      </c>
+      <c r="S316">
+        <v>0.09184902725325056</v>
+      </c>
+      <c r="T316">
+        <v>-0.03597575332675242</v>
+      </c>
+      <c r="U316">
+        <v>0.6883468614234403</v>
+      </c>
+      <c r="V316">
+        <v>-0.5830662405949312</v>
+      </c>
+      <c r="W316">
+        <v>0.2517371917493245</v>
+      </c>
+      <c r="X316">
+        <v>0.06337161370983614</v>
+      </c>
+      <c r="Y316">
+        <v>6.670268377719211</v>
+      </c>
+      <c r="Z316">
+        <v>10.26945576906016</v>
+      </c>
+      <c r="AA316">
+        <v>11.47054488679592</v>
+      </c>
+      <c r="AB316">
+        <v>7.890145752772885</v>
+      </c>
+      <c r="AC316">
+        <v>0.7060355472904661</v>
+      </c>
+      <c r="AD316">
+        <v>0.6554452427947576</v>
+      </c>
+      <c r="AE316">
+        <v>218.7383828256192</v>
+      </c>
+      <c r="AF316">
+        <v>-243.9504001471399</v>
+      </c>
+      <c r="AG316">
+        <v>51.17677876149918</v>
+      </c>
+      <c r="AH316">
+        <v>28.06596829221181</v>
+      </c>
+      <c r="AI316">
+        <v>-0.02985495505010021</v>
+      </c>
+      <c r="AJ316">
+        <v>3.500261584496782</v>
+      </c>
+      <c r="AK316">
+        <v>0.007352941176470588</v>
+      </c>
+      <c r="AL316">
+        <v>0.007352941176470588</v>
+      </c>
+      <c r="AM316" s="2">
+        <v>37729</v>
+      </c>
+      <c r="AN316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:40">
+      <c r="A317" s="1">
+        <v>0</v>
+      </c>
+      <c r="B317" t="s">
+        <v>66</v>
+      </c>
+      <c r="C317">
+        <v>498</v>
+      </c>
+      <c r="D317">
+        <v>14</v>
+      </c>
+      <c r="E317">
+        <v>120.7928973237539</v>
+      </c>
+      <c r="F317">
+        <v>167.7669557925381</v>
+      </c>
+      <c r="G317">
+        <v>-2.463280255804372</v>
+      </c>
+      <c r="H317">
+        <v>53.17188816409772</v>
+      </c>
+      <c r="I317">
+        <v>2827.249690935315</v>
+      </c>
+      <c r="J317">
+        <v>25.04064530493359</v>
+      </c>
+      <c r="K317">
+        <v>54.33478099915746</v>
+      </c>
+      <c r="L317">
+        <v>-0.7877875114846944</v>
+      </c>
+      <c r="M317">
+        <v>17.57783848625664</v>
+      </c>
+      <c r="N317">
+        <v>308.9804058489252</v>
+      </c>
+      <c r="O317">
+        <v>0.3182246293888616</v>
+      </c>
+      <c r="P317">
+        <v>13.87065400784959</v>
+      </c>
+      <c r="Q317">
+        <v>-2.514552597034736</v>
+      </c>
+      <c r="R317">
+        <v>1.619979026692158</v>
+      </c>
+      <c r="S317">
+        <v>2.624332046922472</v>
+      </c>
+      <c r="T317">
+        <v>0.01372137401399066</v>
+      </c>
+      <c r="U317">
+        <v>2.299318538834012</v>
+      </c>
+      <c r="V317">
+        <v>-3.913944584935635</v>
+      </c>
+      <c r="W317">
+        <v>0.7618329459915956</v>
+      </c>
+      <c r="X317">
+        <v>0.5803894375982334</v>
+      </c>
+      <c r="Y317">
+        <v>26.25912035074327</v>
+      </c>
+      <c r="Z317">
+        <v>10.38558287930193</v>
+      </c>
+      <c r="AA317">
+        <v>18.23749434544121</v>
+      </c>
+      <c r="AB317">
+        <v>0</v>
+      </c>
+      <c r="AC317">
+        <v>1.505408105557783</v>
+      </c>
+      <c r="AD317">
+        <v>-1.351184095192497</v>
+      </c>
+      <c r="AE317">
+        <v>840.2655470508188</v>
+      </c>
+      <c r="AF317">
+        <v>-702.8601158091062</v>
+      </c>
+      <c r="AG317">
+        <v>107.739845197138</v>
+      </c>
+      <c r="AH317">
+        <v>52.51031748171807</v>
+      </c>
+      <c r="AI317">
+        <v>0.1858747011840301</v>
+      </c>
+      <c r="AJ317">
+        <v>4.342371043379476</v>
+      </c>
+      <c r="AK317">
+        <v>0.002</v>
+      </c>
+      <c r="AL317">
+        <v>0.002</v>
+      </c>
+      <c r="AM317" s="2">
+        <v>37568</v>
+      </c>
+      <c r="AN317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:40">
+      <c r="A318" s="1">
+        <v>0</v>
+      </c>
+      <c r="B318" t="s">
+        <v>66</v>
+      </c>
+      <c r="C318">
+        <v>498</v>
+      </c>
+      <c r="D318">
+        <v>14</v>
+      </c>
+      <c r="E318">
+        <v>148.8246601706318</v>
+      </c>
+      <c r="F318">
+        <v>167.1309305532021</v>
+      </c>
+      <c r="G318">
+        <v>137.303695589357</v>
+      </c>
+      <c r="H318">
+        <v>6.352667447985388</v>
+      </c>
+      <c r="I318">
+        <v>40.35638370469318</v>
+      </c>
+      <c r="J318">
+        <v>43.31105270729918</v>
+      </c>
+      <c r="K318">
+        <v>59.63772042676757</v>
+      </c>
+      <c r="L318">
+        <v>10.16449949150309</v>
+      </c>
+      <c r="M318">
+        <v>9.874637555524881</v>
+      </c>
+      <c r="N318">
+        <v>97.50846685298239</v>
+      </c>
+      <c r="O318">
+        <v>-0.02032472689418067</v>
+      </c>
+      <c r="P318">
+        <v>3.418020292475035</v>
+      </c>
+      <c r="Q318">
+        <v>-2.912317143942289</v>
+      </c>
+      <c r="R318">
+        <v>0.833141527851501</v>
+      </c>
+      <c r="S318">
+        <v>0.6941248054307334</v>
+      </c>
+      <c r="T318">
+        <v>0.06794420836359691</v>
+      </c>
+      <c r="U318">
+        <v>3.521064564685531</v>
+      </c>
+      <c r="V318">
+        <v>-3.089166879279986</v>
+      </c>
+      <c r="W318">
+        <v>0.9198472850394698</v>
+      </c>
+      <c r="X318">
+        <v>0.8461190277944836</v>
+      </c>
+      <c r="Y318">
+        <v>48.61881241158799</v>
+      </c>
+      <c r="Z318">
+        <v>10.50676488826776</v>
+      </c>
+      <c r="AA318">
+        <v>23.55828092200278</v>
+      </c>
+      <c r="AB318">
+        <v>5.303413994777326</v>
+      </c>
+      <c r="AC318">
+        <v>1.848744464455155</v>
+      </c>
+      <c r="AD318">
+        <v>0.06185307893064754</v>
+      </c>
+      <c r="AE318">
+        <v>1087.487184548957</v>
+      </c>
+      <c r="AF318">
+        <v>-995.5038329162817</v>
+      </c>
+      <c r="AG318">
+        <v>151.3163192606664</v>
+      </c>
+      <c r="AH318">
+        <v>60.05730089187042</v>
+      </c>
+      <c r="AI318">
+        <v>-0.08398404931993304</v>
+      </c>
+      <c r="AJ318">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK318">
+        <v>0.002</v>
+      </c>
+      <c r="AL318">
+        <v>0.002</v>
+      </c>
+      <c r="AM318" s="2">
+        <v>37568</v>
+      </c>
+      <c r="AN318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:40">
+      <c r="A319" s="1">
+        <v>0</v>
+      </c>
+      <c r="B319" t="s">
+        <v>66</v>
+      </c>
+      <c r="C319">
+        <v>498</v>
+      </c>
+      <c r="D319">
+        <v>14</v>
+      </c>
+      <c r="E319">
+        <v>159.7161846180108</v>
+      </c>
+      <c r="F319">
+        <v>171.5909538295842</v>
+      </c>
+      <c r="G319">
+        <v>148.5880185131223</v>
+      </c>
+      <c r="H319">
+        <v>4.375745555449124</v>
+      </c>
+      <c r="I319">
+        <v>19.14714916603277</v>
+      </c>
+      <c r="J319">
+        <v>47.38047913114235</v>
+      </c>
+      <c r="K319">
+        <v>57.51973934912098</v>
+      </c>
+      <c r="L319">
+        <v>34.88133633492613</v>
+      </c>
+      <c r="M319">
+        <v>3.98786842927131</v>
+      </c>
+      <c r="N319">
+        <v>15.90309460917882</v>
+      </c>
+      <c r="O319">
+        <v>0.02254163905790469</v>
+      </c>
+      <c r="P319">
+        <v>2.934482256993448</v>
+      </c>
+      <c r="Q319">
+        <v>-1.982264210132001</v>
+      </c>
+      <c r="R319">
+        <v>0.6550864175778534</v>
+      </c>
+      <c r="S319">
+        <v>0.4291382144949856</v>
+      </c>
+      <c r="T319">
+        <v>-0.002259714363893676</v>
+      </c>
+      <c r="U319">
+        <v>2.124498636461738</v>
+      </c>
+      <c r="V319">
+        <v>-2.171342810917309</v>
+      </c>
+      <c r="W319">
+        <v>0.6857983763914347</v>
+      </c>
+      <c r="X319">
+        <v>0.470319413061128</v>
+      </c>
+      <c r="Y319">
+        <v>48.65307647697489</v>
+      </c>
+      <c r="Z319">
+        <v>10.30106743824449</v>
+      </c>
+      <c r="AA319">
+        <v>17.47732531024127</v>
+      </c>
+      <c r="AB319">
+        <v>4.311159936722366</v>
+      </c>
+      <c r="AC319">
+        <v>1.241759383081121</v>
+      </c>
+      <c r="AD319">
+        <v>-0.3401220564859941</v>
+      </c>
+      <c r="AE319">
+        <v>700.6862252467039</v>
+      </c>
+      <c r="AF319">
+        <v>-770.8260858063641</v>
+      </c>
+      <c r="AG319">
+        <v>101.0972017684026</v>
+      </c>
+      <c r="AH319">
+        <v>39.65645197636665</v>
+      </c>
+      <c r="AI319">
+        <v>-1.13727490935793</v>
+      </c>
+      <c r="AJ319">
+        <v>4.354751391208961</v>
+      </c>
+      <c r="AK319">
+        <v>0.002</v>
+      </c>
+      <c r="AL319">
+        <v>0.002</v>
+      </c>
+      <c r="AM319" s="2">
+        <v>37568</v>
+      </c>
+      <c r="AN319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:40">
+      <c r="A320" s="1">
+        <v>0</v>
+      </c>
+      <c r="B320" t="s">
+        <v>66</v>
+      </c>
+      <c r="C320">
+        <v>498</v>
+      </c>
+      <c r="D320">
+        <v>14</v>
+      </c>
+      <c r="E320">
+        <v>158.1412044322755</v>
+      </c>
+      <c r="F320">
+        <v>169.1589338304992</v>
+      </c>
+      <c r="G320">
+        <v>151.8485584349554</v>
+      </c>
+      <c r="H320">
+        <v>2.90120467639768</v>
+      </c>
+      <c r="I320">
+        <v>8.41698857435177</v>
+      </c>
+      <c r="J320">
+        <v>48.93131921949194</v>
+      </c>
+      <c r="K320">
+        <v>59.10213437145998</v>
+      </c>
+      <c r="L320">
+        <v>34.45570323454264</v>
+      </c>
+      <c r="M320">
+        <v>3.502931004714671</v>
+      </c>
+      <c r="N320">
+        <v>12.27052562379133</v>
+      </c>
+      <c r="O320">
+        <v>-0.01458557521901841</v>
+      </c>
+      <c r="P320">
+        <v>2.045808153908069</v>
+      </c>
+      <c r="Q320">
+        <v>-2.647438251944777</v>
+      </c>
+      <c r="R320">
+        <v>0.6889561847919132</v>
+      </c>
+      <c r="S320">
+        <v>0.4746606245630289</v>
+      </c>
+      <c r="T320">
+        <v>0.0212027440117284</v>
+      </c>
+      <c r="U320">
+        <v>2.973120901307482</v>
+      </c>
+      <c r="V320">
+        <v>-3.790026516019537</v>
+      </c>
+      <c r="W320">
+        <v>0.7725701547792692</v>
+      </c>
+      <c r="X320">
+        <v>0.596864644055664</v>
+      </c>
+      <c r="Y320">
+        <v>49.82457443776205</v>
+      </c>
+      <c r="Z320">
+        <v>10.40299786265609</v>
+      </c>
+      <c r="AA320">
+        <v>20.58289824101553</v>
+      </c>
+      <c r="AB320">
+        <v>5.798974047191451</v>
+      </c>
+      <c r="AC320">
+        <v>1.370074917708267</v>
+      </c>
+      <c r="AD320">
+        <v>-0.2936849028838177</v>
+      </c>
+      <c r="AE320">
+        <v>603.6295149317273</v>
+      </c>
+      <c r="AF320">
+        <v>-893.5114684388124</v>
+      </c>
+      <c r="AG320">
+        <v>91.20339494248584</v>
+      </c>
+      <c r="AH320">
+        <v>33.11036159455946</v>
+      </c>
+      <c r="AI320">
+        <v>-2.975983237696247</v>
+      </c>
+      <c r="AJ320">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK320">
+        <v>0.002</v>
+      </c>
+      <c r="AL320">
+        <v>0.002</v>
+      </c>
+      <c r="AM320" s="2">
+        <v>37568</v>
+      </c>
+      <c r="AN320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:40">
+      <c r="A321" s="1">
+        <v>0</v>
+      </c>
+      <c r="B321" t="s">
+        <v>66</v>
+      </c>
+      <c r="C321">
+        <v>498</v>
+      </c>
+      <c r="D321">
+        <v>14</v>
+      </c>
+      <c r="E321">
+        <v>44.65464357232617</v>
+      </c>
+      <c r="F321">
+        <v>179.8999146470733</v>
+      </c>
+      <c r="G321">
+        <v>-179.9666111386998</v>
+      </c>
+      <c r="H321">
+        <v>68.03271656381547</v>
+      </c>
+      <c r="I321">
+        <v>4628.450523052451</v>
+      </c>
+      <c r="J321">
+        <v>12.1882789614707</v>
+      </c>
+      <c r="K321">
+        <v>60.82816456080045</v>
+      </c>
+      <c r="L321">
+        <v>-11.44666265148102</v>
+      </c>
+      <c r="M321">
+        <v>17.18916494945192</v>
+      </c>
+      <c r="N321">
+        <v>295.4673916594663</v>
+      </c>
+      <c r="O321">
+        <v>-0.3030472270003858</v>
+      </c>
+      <c r="P321">
+        <v>359.0825720547085</v>
+      </c>
+      <c r="Q321">
+        <v>-359.47854484324</v>
+      </c>
+      <c r="R321">
+        <v>22.90300531156468</v>
+      </c>
+      <c r="S321">
+        <v>524.5476523015601</v>
+      </c>
+      <c r="T321">
+        <v>-0.1032420143453956</v>
+      </c>
+      <c r="U321">
+        <v>3.290013623036245</v>
+      </c>
+      <c r="V321">
+        <v>-3.135492402591247</v>
+      </c>
+      <c r="W321">
+        <v>0.6664703445183525</v>
+      </c>
+      <c r="X321">
+        <v>0.4441827201224114</v>
+      </c>
+      <c r="Y321">
+        <v>6.481620084047973</v>
+      </c>
+      <c r="Z321">
+        <v>10.26615716334954</v>
+      </c>
+      <c r="AA321">
+        <v>21.84252961540856</v>
+      </c>
+      <c r="AB321">
+        <v>4.871940065312791</v>
+      </c>
+      <c r="AC321">
+        <v>1.852817736458745</v>
+      </c>
+      <c r="AD321">
+        <v>0.2395184532640649</v>
+      </c>
+      <c r="AE321">
+        <v>925.8608666635881</v>
+      </c>
+      <c r="AF321">
+        <v>-741.2384893130395</v>
+      </c>
+      <c r="AG321">
+        <v>118.2744853393295</v>
+      </c>
+      <c r="AH321">
+        <v>39.75551470624522</v>
+      </c>
+      <c r="AI321">
+        <v>0.9243247790257746</v>
+      </c>
+      <c r="AJ321">
+        <v>4.329979584381723</v>
+      </c>
+      <c r="AK321">
+        <v>0.002</v>
+      </c>
+      <c r="AL321">
+        <v>0.002</v>
+      </c>
+      <c r="AM321" s="2">
+        <v>37568</v>
+      </c>
+      <c r="AN321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:40">
+      <c r="A322" s="1">
+        <v>0</v>
+      </c>
+      <c r="B322" t="s">
+        <v>67</v>
+      </c>
+      <c r="C322">
+        <v>509</v>
+      </c>
+      <c r="D322">
+        <v>9</v>
+      </c>
+      <c r="E322">
+        <v>89.6897054376043</v>
+      </c>
+      <c r="F322">
+        <v>150.4354085663379</v>
+      </c>
+      <c r="G322">
+        <v>-4.958133226065067</v>
+      </c>
+      <c r="H322">
+        <v>46.79900244666706</v>
+      </c>
+      <c r="I322">
+        <v>2190.14663000315</v>
+      </c>
+      <c r="J322">
+        <v>38.32889112143368</v>
+      </c>
+      <c r="K322">
+        <v>71.67410976414351</v>
+      </c>
+      <c r="L322">
+        <v>-10.43692102156405</v>
+      </c>
+      <c r="M322">
+        <v>30.36506098185226</v>
+      </c>
+      <c r="N322">
+        <v>922.0369284316066</v>
+      </c>
+      <c r="O322">
+        <v>0.2181110733205438</v>
+      </c>
+      <c r="P322">
+        <v>7.674884801133786</v>
+      </c>
+      <c r="Q322">
+        <v>-10.19143347342462</v>
+      </c>
+      <c r="R322">
+        <v>1.853852911466667</v>
+      </c>
+      <c r="S322">
+        <v>3.436770617353439</v>
+      </c>
+      <c r="T322">
+        <v>0.1256654612872683</v>
+      </c>
+      <c r="U322">
+        <v>3.038059989197478</v>
+      </c>
+      <c r="V322">
+        <v>-2.456928036027477</v>
+      </c>
+      <c r="W322">
+        <v>0.736113647931297</v>
+      </c>
+      <c r="X322">
+        <v>0.5418633026707214</v>
+      </c>
+      <c r="Y322">
+        <v>62.09435945159407</v>
+      </c>
+      <c r="Z322">
+        <v>10.31183052453401</v>
+      </c>
+      <c r="AA322">
+        <v>18.39260177353927</v>
+      </c>
+      <c r="AB322">
+        <v>0</v>
+      </c>
+      <c r="AC322">
+        <v>1.640514983812379</v>
+      </c>
+      <c r="AD322">
+        <v>0.1118081950903427</v>
+      </c>
+      <c r="AE322">
+        <v>634.5946372800078</v>
+      </c>
+      <c r="AF322">
+        <v>-553.2321625473621</v>
+      </c>
+      <c r="AG322">
+        <v>116.2087032285916</v>
+      </c>
+      <c r="AH322">
+        <v>49.93223160541763</v>
+      </c>
+      <c r="AI322">
+        <v>0.5358035668476249</v>
+      </c>
+      <c r="AJ322">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK322">
+        <v>0.002</v>
+      </c>
+      <c r="AL322">
+        <v>0.002</v>
+      </c>
+      <c r="AM322" s="2">
+        <v>37625</v>
+      </c>
+      <c r="AN322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:40">
+      <c r="A323" s="1">
+        <v>0</v>
+      </c>
+      <c r="B323" t="s">
+        <v>67</v>
+      </c>
+      <c r="C323">
+        <v>509</v>
+      </c>
+      <c r="D323">
+        <v>9</v>
+      </c>
+      <c r="E323">
+        <v>116.7484361886414</v>
+      </c>
+      <c r="F323">
+        <v>135.3104863770145</v>
+      </c>
+      <c r="G323">
+        <v>93.2107307973595</v>
+      </c>
+      <c r="H323">
+        <v>7.190483226719741</v>
+      </c>
+      <c r="I323">
+        <v>51.70304903373794</v>
+      </c>
+      <c r="J323">
+        <v>65.81914297512313</v>
+      </c>
+      <c r="K323">
+        <v>75.30288662105454</v>
+      </c>
+      <c r="L323">
+        <v>52.49903681531839</v>
+      </c>
+      <c r="M323">
+        <v>2.79308414858879</v>
+      </c>
+      <c r="N323">
+        <v>7.801319061097964</v>
+      </c>
+      <c r="O323">
+        <v>0.03482209407650105</v>
+      </c>
+      <c r="P323">
+        <v>8.97825586358546</v>
+      </c>
+      <c r="Q323">
+        <v>-6.008262524944229</v>
+      </c>
+      <c r="R323">
+        <v>1.809826022476705</v>
+      </c>
+      <c r="S323">
+        <v>3.275470231633849</v>
+      </c>
+      <c r="T323">
+        <v>0.0119903709511127</v>
+      </c>
+      <c r="U323">
+        <v>2.007546528609197</v>
+      </c>
+      <c r="V323">
+        <v>-2.27470473113749</v>
+      </c>
+      <c r="W323">
+        <v>0.5878927070290769</v>
+      </c>
+      <c r="X323">
+        <v>0.345617834977976</v>
+      </c>
+      <c r="Y323">
+        <v>66.34866333695405</v>
+      </c>
+      <c r="Z323">
+        <v>10.18131450966247</v>
+      </c>
+      <c r="AA323">
+        <v>14.95987633638728</v>
+      </c>
+      <c r="AB323">
+        <v>8.672957972917891</v>
+      </c>
+      <c r="AC323">
+        <v>0.6757060104523552</v>
+      </c>
+      <c r="AD323">
+        <v>-0.1320700659142487</v>
+      </c>
+      <c r="AE323">
+        <v>388.4646883389216</v>
+      </c>
+      <c r="AF323">
+        <v>-351.0450069693378</v>
+      </c>
+      <c r="AG323">
+        <v>59.60380843345217</v>
+      </c>
+      <c r="AH323">
+        <v>25.23384633880364</v>
+      </c>
+      <c r="AI323">
+        <v>-0.447108629248287</v>
+      </c>
+      <c r="AJ323">
+        <v>4.36712056579597</v>
+      </c>
+      <c r="AK323">
+        <v>0.002</v>
+      </c>
+      <c r="AL323">
+        <v>0.002</v>
+      </c>
+      <c r="AM323" s="2">
+        <v>37625</v>
+      </c>
+      <c r="AN323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:40">
+      <c r="A324" s="1">
+        <v>0</v>
+      </c>
+      <c r="B324" t="s">
+        <v>67</v>
+      </c>
+      <c r="C324">
+        <v>509</v>
+      </c>
+      <c r="D324">
+        <v>9</v>
+      </c>
+      <c r="E324">
+        <v>122.366532534511</v>
+      </c>
+      <c r="F324">
+        <v>156.2003656959804</v>
+      </c>
+      <c r="G324">
+        <v>102.3360326833501</v>
+      </c>
+      <c r="H324">
+        <v>8.280207624047842</v>
+      </c>
+      <c r="I324">
+        <v>68.56183829734002</v>
+      </c>
+      <c r="J324">
+        <v>65.0163677736211</v>
+      </c>
+      <c r="K324">
+        <v>75.94701358176036</v>
+      </c>
+      <c r="L324">
+        <v>40.62065288722485</v>
+      </c>
+      <c r="M324">
+        <v>5.044831314751825</v>
+      </c>
+      <c r="N324">
+        <v>25.45032299430062</v>
+      </c>
+      <c r="O324">
+        <v>0.01000966525903377</v>
+      </c>
+      <c r="P324">
+        <v>8.337605106542924</v>
+      </c>
+      <c r="Q324">
+        <v>-15.83869417817002</v>
+      </c>
+      <c r="R324">
+        <v>2.071743225268199</v>
+      </c>
+      <c r="S324">
+        <v>4.292119991444681</v>
+      </c>
+      <c r="T324">
+        <v>-0.003249590318725854</v>
+      </c>
+      <c r="U324">
+        <v>3.104530459169155</v>
+      </c>
+      <c r="V324">
+        <v>-3.272415722930077</v>
+      </c>
+      <c r="W324">
+        <v>0.6479903317991688</v>
+      </c>
+      <c r="X324">
+        <v>0.4198914701051968</v>
+      </c>
+      <c r="Y324">
+        <v>66.54951232347554</v>
+      </c>
+      <c r="Z324">
+        <v>10.19989958302781</v>
+      </c>
+      <c r="AA324">
+        <v>21.72595452448522</v>
+      </c>
+      <c r="AB324">
+        <v>7.272317374812515</v>
+      </c>
+      <c r="AC324">
+        <v>1.000693895601765</v>
+      </c>
+      <c r="AD324">
+        <v>0.2960262348093964</v>
+      </c>
+      <c r="AE324">
+        <v>968.9661059409391</v>
+      </c>
+      <c r="AF324">
+        <v>-659.0524677730835</v>
+      </c>
+      <c r="AG324">
+        <v>78.84379220028161</v>
+      </c>
+      <c r="AH324">
+        <v>26.84333092099724</v>
+      </c>
+      <c r="AI324">
+        <v>2.613510025581566</v>
+      </c>
+      <c r="AJ324">
+        <v>4.317577075603999</v>
+      </c>
+      <c r="AK324">
+        <v>0.002</v>
+      </c>
+      <c r="AL324">
+        <v>0.002</v>
+      </c>
+      <c r="AM324" s="2">
+        <v>37625</v>
+      </c>
+      <c r="AN324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:40">
+      <c r="A325" s="1">
+        <v>0</v>
+      </c>
+      <c r="B325" t="s">
+        <v>67</v>
+      </c>
+      <c r="C325">
+        <v>509</v>
+      </c>
+      <c r="D325">
+        <v>9</v>
+      </c>
+      <c r="E325">
+        <v>97.78262343980968</v>
+      </c>
+      <c r="F325">
+        <v>165.3119080729498</v>
+      </c>
+      <c r="G325">
+        <v>7.962330555272269</v>
+      </c>
+      <c r="H325">
+        <v>54.51303795485094</v>
+      </c>
+      <c r="I325">
+        <v>2971.671307067018</v>
+      </c>
+      <c r="J325">
+        <v>47.22395495440888</v>
+      </c>
+      <c r="K325">
+        <v>77.43701279684893</v>
+      </c>
+      <c r="L325">
+        <v>0.6128896697946686</v>
+      </c>
+      <c r="M325">
+        <v>27.30943759056663</v>
+      </c>
+      <c r="N325">
+        <v>745.8053815130536</v>
+      </c>
+      <c r="O325">
+        <v>-0.2312918760729922</v>
+      </c>
+      <c r="P325">
+        <v>7.205657281115663</v>
+      </c>
+      <c r="Q325">
+        <v>-7.556265483419907</v>
+      </c>
+      <c r="R325">
+        <v>1.751539296377467</v>
+      </c>
+      <c r="S325">
+        <v>3.067889906754473</v>
+      </c>
+      <c r="T325">
+        <v>-0.1373176411256559</v>
+      </c>
+      <c r="U325">
+        <v>1.75878240038756</v>
+      </c>
+      <c r="V325">
+        <v>-3.897959341911054</v>
+      </c>
+      <c r="W325">
+        <v>0.6804337244922393</v>
+      </c>
+      <c r="X325">
+        <v>0.4629900534263806</v>
+      </c>
+      <c r="Y325">
+        <v>64.900064407787</v>
+      </c>
+      <c r="Z325">
+        <v>10.11163138015587</v>
+      </c>
+      <c r="AA325">
+        <v>17.3433128323282</v>
+      </c>
+      <c r="AB325">
+        <v>5.720673037326989</v>
+      </c>
+      <c r="AC325">
+        <v>1.116778142105532</v>
+      </c>
+      <c r="AD325">
+        <v>0.2897475222634098</v>
+      </c>
+      <c r="AE325">
+        <v>501.8095004422596</v>
+      </c>
+      <c r="AF325">
+        <v>-700.6204438975719</v>
+      </c>
+      <c r="AG325">
+        <v>75.76661109427236</v>
+      </c>
+      <c r="AH325">
+        <v>28.95549665220186</v>
+      </c>
+      <c r="AI325">
+        <v>-1.00448963194182</v>
+      </c>
+      <c r="AJ325">
+        <v>4.305163577759991</v>
+      </c>
+      <c r="AK325">
+        <v>0.002</v>
+      </c>
+      <c r="AL325">
+        <v>0.002</v>
+      </c>
+      <c r="AM325" s="2">
+        <v>37625</v>
+      </c>
+      <c r="AN325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:40">
+      <c r="A326" s="1">
+        <v>0</v>
+      </c>
+      <c r="B326" t="s">
+        <v>67</v>
+      </c>
+      <c r="C326">
+        <v>509</v>
+      </c>
+      <c r="D326">
+        <v>9</v>
+      </c>
+      <c r="E326">
+        <v>18.82691244781045</v>
+      </c>
+      <c r="F326">
+        <v>20.26059085445424</v>
+      </c>
+      <c r="G326">
+        <v>16.57970419764393</v>
+      </c>
+      <c r="H326">
+        <v>0.9263404728453565</v>
+      </c>
+      <c r="I326">
+        <v>0.8581066716313587</v>
+      </c>
+      <c r="J326">
+        <v>0.9584965342575359</v>
+      </c>
+      <c r="K326">
+        <v>1.283063570206565</v>
+      </c>
+      <c r="L326">
+        <v>0.6266217622086572</v>
+      </c>
+      <c r="M326">
+        <v>0.2269672491911777</v>
+      </c>
+      <c r="N326">
+        <v>0.05151413220541016</v>
+      </c>
+      <c r="O326">
+        <v>-0.03179214110401956</v>
+      </c>
+      <c r="P326">
+        <v>0.615664157294681</v>
+      </c>
+      <c r="Q326">
+        <v>-0.3924236518218898</v>
+      </c>
+      <c r="R326">
+        <v>0.2351674799773378</v>
+      </c>
+      <c r="S326">
+        <v>0.05530374363889155</v>
+      </c>
+      <c r="T326">
+        <v>0.01158835598140848</v>
+      </c>
+      <c r="U326">
+        <v>0.3084164759108176</v>
+      </c>
+      <c r="V326">
+        <v>-0.2947745195302359</v>
+      </c>
+      <c r="W326">
+        <v>0.09864364192355159</v>
+      </c>
+      <c r="X326">
+        <v>0.009730568091941864</v>
+      </c>
+      <c r="Y326">
+        <v>1.067828295391632</v>
+      </c>
+      <c r="Z326">
+        <v>9.940879351210372</v>
+      </c>
+      <c r="AA326">
+        <v>10.62540822745178</v>
+      </c>
+      <c r="AB326">
+        <v>9.441281692651692</v>
+      </c>
+      <c r="AC326">
+        <v>0.2144885979378409</v>
+      </c>
+      <c r="AD326">
+        <v>-0.01069149800096705</v>
+      </c>
+      <c r="AE326">
+        <v>79.78018168577164</v>
+      </c>
+      <c r="AF326">
+        <v>-98.67721123333706</v>
+      </c>
+      <c r="AG326">
+        <v>25.74971377767432</v>
+      </c>
+      <c r="AH326">
+        <v>10.89323044383167</v>
+      </c>
+      <c r="AI326">
+        <v>-0.2431263191399824</v>
+      </c>
+      <c r="AJ326">
+        <v>2.82061355391094</v>
+      </c>
+      <c r="AK326">
+        <v>0.025</v>
+      </c>
+      <c r="AL326">
+        <v>0.025</v>
+      </c>
+      <c r="AM326" s="2">
+        <v>37625</v>
+      </c>
+      <c r="AN326">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>